<commit_message>
Updated title for neonatal mortality
</commit_message>
<xml_diff>
--- a/data/MDG Data.xlsx
+++ b/data/MDG Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="999" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="999" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Proposed Indicators" sheetId="7" r:id="rId1"/>
@@ -8354,6 +8354,71 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="166" fontId="36" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="23" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="38" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="39" fillId="0" borderId="0" xfId="23" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -8381,46 +8446,40 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8432,73 +8491,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="36" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="23" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="38" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="39" fillId="0" borderId="0" xfId="23" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="92">
@@ -9232,11 +9232,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2089218568"/>
-        <c:axId val="2089218920"/>
+        <c:axId val="-2143166440"/>
+        <c:axId val="-2142767176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2089218568"/>
+        <c:axId val="-2143166440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9245,7 +9245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089218920"/>
+        <c:crossAx val="-2142767176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9253,7 +9253,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2089218920"/>
+        <c:axId val="-2142767176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9264,7 +9264,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089218568"/>
+        <c:crossAx val="-2143166440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9431,11 +9431,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125398248"/>
-        <c:axId val="2125394184"/>
+        <c:axId val="-2142819880"/>
+        <c:axId val="-2142816808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125398248"/>
+        <c:axId val="-2142819880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9445,7 +9445,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125394184"/>
+        <c:crossAx val="-2142816808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9453,7 +9453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125394184"/>
+        <c:axId val="-2142816808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9464,7 +9464,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125398248"/>
+        <c:crossAx val="-2142819880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9695,11 +9695,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2143024696"/>
-        <c:axId val="-2142856328"/>
+        <c:axId val="-2141825720"/>
+        <c:axId val="-2143175032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2143024696"/>
+        <c:axId val="-2141825720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9709,7 +9709,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142856328"/>
+        <c:crossAx val="-2143175032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9717,7 +9717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2142856328"/>
+        <c:axId val="-2143175032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9728,7 +9728,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143024696"/>
+        <c:crossAx val="-2141825720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9862,11 +9862,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2127166008"/>
-        <c:axId val="2127168952"/>
+        <c:axId val="-2143204120"/>
+        <c:axId val="-2143235416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127166008"/>
+        <c:axId val="-2143204120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9875,7 +9875,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127168952"/>
+        <c:crossAx val="-2143235416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9883,7 +9883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127168952"/>
+        <c:axId val="-2143235416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9894,7 +9894,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127166008"/>
+        <c:crossAx val="-2143204120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10056,11 +10056,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127216344"/>
-        <c:axId val="2127219432"/>
+        <c:axId val="-2142390072"/>
+        <c:axId val="-2142989416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127216344"/>
+        <c:axId val="-2142390072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10070,7 +10070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127219432"/>
+        <c:crossAx val="-2142989416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10078,7 +10078,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127219432"/>
+        <c:axId val="-2142989416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10089,7 +10089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127216344"/>
+        <c:crossAx val="-2142390072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -32868,10 +32868,10 @@
     <row r="4" spans="1:8">
       <c r="A4" s="20"/>
       <c r="B4" s="104"/>
-      <c r="C4" s="159" t="s">
+      <c r="C4" s="140" t="s">
         <v>2379</v>
       </c>
-      <c r="D4" s="159" t="s">
+      <c r="D4" s="140" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="107"/>
@@ -32884,8 +32884,8 @@
       <c r="B5" s="105" t="s">
         <v>2378</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="141"/>
       <c r="E5" s="108">
         <v>2011</v>
       </c>
@@ -32902,8 +32902,8 @@
     <row r="6" spans="1:8" ht="16" thickBot="1">
       <c r="A6" s="20"/>
       <c r="B6" s="106"/>
-      <c r="C6" s="161"/>
-      <c r="D6" s="161"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="142"/>
       <c r="E6" s="109"/>
       <c r="F6" s="109"/>
       <c r="G6" s="109"/>
@@ -32955,57 +32955,57 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="20"/>
-      <c r="B9" s="120"/>
-      <c r="C9" s="121"/>
-      <c r="D9" s="121"/>
-      <c r="E9" s="121"/>
-      <c r="F9" s="121"/>
-      <c r="G9" s="121"/>
-      <c r="H9" s="122"/>
+      <c r="B9" s="143"/>
+      <c r="C9" s="144"/>
+      <c r="D9" s="144"/>
+      <c r="E9" s="144"/>
+      <c r="F9" s="144"/>
+      <c r="G9" s="144"/>
+      <c r="H9" s="145"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="20"/>
-      <c r="B10" s="123" t="s">
+      <c r="B10" s="146" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="124"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="125"/>
+      <c r="C10" s="147"/>
+      <c r="D10" s="147"/>
+      <c r="E10" s="147"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="147"/>
+      <c r="H10" s="148"/>
     </row>
     <row r="11" spans="1:8" ht="16" thickBot="1">
       <c r="A11" s="20"/>
-      <c r="B11" s="126"/>
-      <c r="C11" s="127"/>
-      <c r="D11" s="127"/>
-      <c r="E11" s="127"/>
-      <c r="F11" s="127"/>
-      <c r="G11" s="127"/>
-      <c r="H11" s="128"/>
+      <c r="B11" s="149"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="150"/>
+      <c r="F11" s="150"/>
+      <c r="G11" s="150"/>
+      <c r="H11" s="151"/>
     </row>
     <row r="12" spans="1:8" ht="39" customHeight="1">
       <c r="A12" s="20"/>
       <c r="B12" s="3" t="s">
         <v>2380</v>
       </c>
-      <c r="C12" s="137" t="s">
+      <c r="C12" s="127" t="s">
         <v>2382</v>
       </c>
-      <c r="D12" s="137" t="s">
+      <c r="D12" s="127" t="s">
         <v>2383</v>
       </c>
-      <c r="E12" s="153">
+      <c r="E12" s="155">
         <v>0.29699999999999999</v>
       </c>
-      <c r="F12" s="137" t="s">
+      <c r="F12" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="137" t="s">
+      <c r="G12" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="137" t="s">
+      <c r="H12" s="127" t="s">
         <v>24</v>
       </c>
     </row>
@@ -33014,34 +33014,34 @@
       <c r="B13" s="1" t="s">
         <v>2381</v>
       </c>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="154"/>
-      <c r="F13" s="138"/>
-      <c r="G13" s="138"/>
-      <c r="H13" s="138"/>
+      <c r="C13" s="129"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="156"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="129"/>
+      <c r="H13" s="129"/>
     </row>
     <row r="14" spans="1:8" ht="39" customHeight="1">
       <c r="A14" s="20"/>
       <c r="B14" s="3" t="s">
         <v>2384</v>
       </c>
-      <c r="C14" s="137" t="s">
+      <c r="C14" s="127" t="s">
         <v>2382</v>
       </c>
-      <c r="D14" s="137" t="s">
+      <c r="D14" s="127" t="s">
         <v>2385</v>
       </c>
-      <c r="E14" s="153">
+      <c r="E14" s="155">
         <v>0.10199999999999999</v>
       </c>
-      <c r="F14" s="137" t="s">
+      <c r="F14" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="137" t="s">
+      <c r="G14" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="137" t="s">
+      <c r="H14" s="127" t="s">
         <v>24</v>
       </c>
     </row>
@@ -33050,211 +33050,211 @@
       <c r="B15" s="1" t="s">
         <v>2381</v>
       </c>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="154"/>
-      <c r="F15" s="138"/>
-      <c r="G15" s="138"/>
-      <c r="H15" s="138"/>
+      <c r="C15" s="129"/>
+      <c r="D15" s="129"/>
+      <c r="E15" s="156"/>
+      <c r="F15" s="129"/>
+      <c r="G15" s="129"/>
+      <c r="H15" s="129"/>
     </row>
     <row r="16" spans="1:8" ht="74" customHeight="1">
       <c r="A16" s="20"/>
-      <c r="B16" s="139" t="s">
+      <c r="B16" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="137" t="s">
+      <c r="C16" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="150" t="s">
+      <c r="D16" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="137">
+      <c r="E16" s="127">
         <v>32.799999999999997</v>
       </c>
-      <c r="F16" s="137" t="s">
+      <c r="F16" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="137" t="s">
+      <c r="G16" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="137" t="s">
+      <c r="H16" s="127" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="16" thickBot="1">
       <c r="A17" s="20"/>
-      <c r="B17" s="141"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="152"/>
-      <c r="E17" s="138"/>
-      <c r="F17" s="138"/>
-      <c r="G17" s="138"/>
-      <c r="H17" s="138"/>
+      <c r="B17" s="126"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="159"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="129"/>
+      <c r="G17" s="129"/>
+      <c r="H17" s="129"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="20"/>
-      <c r="B18" s="129" t="s">
+      <c r="B18" s="136" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="133" t="s">
+      <c r="D18" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="135">
+      <c r="E18" s="130">
         <v>-1.73</v>
       </c>
-      <c r="F18" s="135">
+      <c r="F18" s="130">
         <v>-2.37</v>
       </c>
-      <c r="G18" s="135" t="s">
+      <c r="G18" s="130" t="s">
         <v>2387</v>
       </c>
-      <c r="H18" s="135" t="s">
+      <c r="H18" s="130" t="s">
         <v>2387</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="22">
       <c r="A19" s="20"/>
-      <c r="B19" s="146"/>
+      <c r="B19" s="137"/>
       <c r="C19" s="6" t="s">
         <v>2386</v>
       </c>
-      <c r="D19" s="156"/>
-      <c r="E19" s="147"/>
-      <c r="F19" s="147"/>
-      <c r="G19" s="147"/>
-      <c r="H19" s="147"/>
+      <c r="D19" s="157"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="139"/>
+      <c r="H19" s="139"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="20"/>
-      <c r="B20" s="146"/>
+      <c r="B20" s="137"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="147"/>
-      <c r="F20" s="147"/>
-      <c r="G20" s="147"/>
-      <c r="H20" s="147"/>
+      <c r="D20" s="157"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="139"/>
+      <c r="H20" s="139"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="20"/>
-      <c r="B21" s="146"/>
+      <c r="B21" s="137"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="156"/>
-      <c r="E21" s="147"/>
-      <c r="F21" s="147"/>
-      <c r="G21" s="147"/>
-      <c r="H21" s="147"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="139"/>
+      <c r="H21" s="139"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="20"/>
-      <c r="B22" s="146"/>
+      <c r="B22" s="137"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="156"/>
-      <c r="E22" s="147"/>
-      <c r="F22" s="147"/>
-      <c r="G22" s="147"/>
-      <c r="H22" s="147"/>
+      <c r="D22" s="157"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="139"/>
     </row>
     <row r="23" spans="1:8" ht="16" thickBot="1">
       <c r="A23" s="20"/>
-      <c r="B23" s="130"/>
+      <c r="B23" s="138"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="134"/>
-      <c r="E23" s="136"/>
-      <c r="F23" s="136"/>
-      <c r="G23" s="136"/>
-      <c r="H23" s="136"/>
+      <c r="D23" s="133"/>
+      <c r="E23" s="131"/>
+      <c r="F23" s="131"/>
+      <c r="G23" s="131"/>
+      <c r="H23" s="131"/>
     </row>
     <row r="24" spans="1:8" ht="17" customHeight="1">
       <c r="A24" s="20"/>
-      <c r="B24" s="129" t="s">
+      <c r="B24" s="136" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="157" t="s">
+      <c r="D24" s="160" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="135">
+      <c r="E24" s="130">
         <v>7.3</v>
       </c>
-      <c r="F24" s="135">
+      <c r="F24" s="130">
         <v>2.5</v>
       </c>
-      <c r="G24" s="135">
+      <c r="G24" s="130">
         <v>1.8</v>
       </c>
-      <c r="H24" s="135" t="s">
+      <c r="H24" s="130" t="s">
         <v>2389</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="16" thickBot="1">
       <c r="A25" s="20"/>
-      <c r="B25" s="130"/>
+      <c r="B25" s="138"/>
       <c r="C25" s="10" t="s">
         <v>2388</v>
       </c>
-      <c r="D25" s="158"/>
-      <c r="E25" s="136"/>
-      <c r="F25" s="136"/>
-      <c r="G25" s="136"/>
-      <c r="H25" s="136"/>
+      <c r="D25" s="161"/>
+      <c r="E25" s="131"/>
+      <c r="F25" s="131"/>
+      <c r="G25" s="131"/>
+      <c r="H25" s="131"/>
     </row>
     <row r="26" spans="1:8" ht="44" customHeight="1">
       <c r="A26" s="20"/>
-      <c r="B26" s="129" t="s">
+      <c r="B26" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="135" t="s">
+      <c r="C26" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="D26" s="133" t="s">
+      <c r="D26" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="135" t="s">
+      <c r="E26" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="135" t="s">
+      <c r="F26" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="135">
+      <c r="G26" s="130">
         <v>0.28000000000000003</v>
       </c>
-      <c r="H26" s="135" t="s">
+      <c r="H26" s="130" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="16" thickBot="1">
       <c r="A27" s="20"/>
-      <c r="B27" s="130"/>
-      <c r="C27" s="136"/>
-      <c r="D27" s="134"/>
-      <c r="E27" s="136"/>
-      <c r="F27" s="136"/>
-      <c r="G27" s="136"/>
-      <c r="H27" s="136"/>
+      <c r="B27" s="138"/>
+      <c r="C27" s="131"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="131"/>
+      <c r="F27" s="131"/>
+      <c r="G27" s="131"/>
+      <c r="H27" s="131"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="20"/>
-      <c r="B28" s="129" t="s">
+      <c r="B28" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="135" t="s">
+      <c r="C28" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="133" t="s">
+      <c r="D28" s="132" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="135" t="s">
+      <c r="E28" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="135" t="s">
+      <c r="F28" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="135" t="s">
+      <c r="G28" s="130" t="s">
         <v>24</v>
       </c>
       <c r="H28" s="6" t="s">
@@ -33263,49 +33263,49 @@
     </row>
     <row r="29" spans="1:8" ht="22">
       <c r="A29" s="20"/>
-      <c r="B29" s="146"/>
-      <c r="C29" s="147"/>
-      <c r="D29" s="156"/>
-      <c r="E29" s="147"/>
-      <c r="F29" s="147"/>
-      <c r="G29" s="147"/>
+      <c r="B29" s="137"/>
+      <c r="C29" s="139"/>
+      <c r="D29" s="157"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="139"/>
       <c r="H29" s="6" t="s">
         <v>2390</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="22">
       <c r="A30" s="20"/>
-      <c r="B30" s="146"/>
-      <c r="C30" s="147"/>
-      <c r="D30" s="156"/>
-      <c r="E30" s="147"/>
-      <c r="F30" s="147"/>
-      <c r="G30" s="147"/>
+      <c r="B30" s="137"/>
+      <c r="C30" s="139"/>
+      <c r="D30" s="157"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="139"/>
       <c r="H30" s="6" t="s">
         <v>2391</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="16" thickBot="1">
       <c r="A31" s="20"/>
-      <c r="B31" s="130"/>
-      <c r="C31" s="136"/>
-      <c r="D31" s="134"/>
-      <c r="E31" s="136"/>
-      <c r="F31" s="136"/>
-      <c r="G31" s="136"/>
+      <c r="B31" s="138"/>
+      <c r="C31" s="131"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="131"/>
+      <c r="F31" s="131"/>
+      <c r="G31" s="131"/>
       <c r="H31" s="10" t="s">
         <v>2392</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="22">
       <c r="A32" s="20"/>
-      <c r="B32" s="129" t="s">
+      <c r="B32" s="136" t="s">
         <v>2393</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="133" t="s">
+      <c r="D32" s="132" t="s">
         <v>35</v>
       </c>
       <c r="E32" s="6" t="s">
@@ -33323,11 +33323,11 @@
     </row>
     <row r="33" spans="1:8" ht="22">
       <c r="A33" s="20"/>
-      <c r="B33" s="146"/>
+      <c r="B33" s="137"/>
       <c r="C33" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="156"/>
+      <c r="D33" s="157"/>
       <c r="E33" s="6" t="s">
         <v>2396</v>
       </c>
@@ -33343,11 +33343,11 @@
     </row>
     <row r="34" spans="1:8" ht="55">
       <c r="A34" s="20"/>
-      <c r="B34" s="146"/>
+      <c r="B34" s="137"/>
       <c r="C34" s="6" t="s">
         <v>2394</v>
       </c>
-      <c r="D34" s="156"/>
+      <c r="D34" s="157"/>
       <c r="E34" s="6" t="s">
         <v>2397</v>
       </c>
@@ -33363,11 +33363,11 @@
     </row>
     <row r="35" spans="1:8" ht="66">
       <c r="A35" s="20"/>
-      <c r="B35" s="146"/>
+      <c r="B35" s="137"/>
       <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="156"/>
+      <c r="D35" s="157"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
@@ -33377,9 +33377,9 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="20"/>
-      <c r="B36" s="146"/>
+      <c r="B36" s="137"/>
       <c r="C36" s="6"/>
-      <c r="D36" s="156"/>
+      <c r="D36" s="157"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -33387,9 +33387,9 @@
     </row>
     <row r="37" spans="1:8" ht="16" thickBot="1">
       <c r="A37" s="20"/>
-      <c r="B37" s="130"/>
+      <c r="B37" s="138"/>
       <c r="C37" s="10"/>
-      <c r="D37" s="134"/>
+      <c r="D37" s="133"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
@@ -33419,90 +33419,90 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="20"/>
-      <c r="B39" s="120"/>
-      <c r="C39" s="121"/>
-      <c r="D39" s="121"/>
-      <c r="E39" s="121"/>
-      <c r="F39" s="121"/>
-      <c r="G39" s="121"/>
-      <c r="H39" s="122"/>
+      <c r="B39" s="143"/>
+      <c r="C39" s="144"/>
+      <c r="D39" s="144"/>
+      <c r="E39" s="144"/>
+      <c r="F39" s="144"/>
+      <c r="G39" s="144"/>
+      <c r="H39" s="145"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="20"/>
-      <c r="B40" s="123" t="s">
+      <c r="B40" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="124"/>
-      <c r="D40" s="124"/>
-      <c r="E40" s="124"/>
-      <c r="F40" s="124"/>
-      <c r="G40" s="124"/>
-      <c r="H40" s="125"/>
+      <c r="C40" s="147"/>
+      <c r="D40" s="147"/>
+      <c r="E40" s="147"/>
+      <c r="F40" s="147"/>
+      <c r="G40" s="147"/>
+      <c r="H40" s="148"/>
     </row>
     <row r="41" spans="1:8" ht="16" thickBot="1">
       <c r="A41" s="20"/>
-      <c r="B41" s="126"/>
-      <c r="C41" s="127"/>
-      <c r="D41" s="127"/>
-      <c r="E41" s="127"/>
-      <c r="F41" s="127"/>
-      <c r="G41" s="127"/>
-      <c r="H41" s="128"/>
+      <c r="B41" s="149"/>
+      <c r="C41" s="150"/>
+      <c r="D41" s="150"/>
+      <c r="E41" s="150"/>
+      <c r="F41" s="150"/>
+      <c r="G41" s="150"/>
+      <c r="H41" s="151"/>
     </row>
     <row r="42" spans="1:8" ht="39" customHeight="1">
       <c r="A42" s="20"/>
-      <c r="B42" s="139" t="s">
+      <c r="B42" s="124" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="137" t="s">
+      <c r="C42" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="D42" s="137" t="s">
+      <c r="D42" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="137" t="s">
+      <c r="E42" s="127" t="s">
         <v>40</v>
       </c>
       <c r="F42" s="4">
         <v>36.9</v>
       </c>
-      <c r="G42" s="153">
+      <c r="G42" s="155">
         <v>0.40500000000000003</v>
       </c>
-      <c r="H42" s="137" t="s">
+      <c r="H42" s="127" t="s">
         <v>2406</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="16" thickBot="1">
       <c r="A43" s="20"/>
-      <c r="B43" s="141"/>
-      <c r="C43" s="138"/>
-      <c r="D43" s="138"/>
-      <c r="E43" s="138"/>
+      <c r="B43" s="126"/>
+      <c r="C43" s="129"/>
+      <c r="D43" s="129"/>
+      <c r="E43" s="129"/>
       <c r="F43" s="2" t="s">
         <v>2405</v>
       </c>
-      <c r="G43" s="154"/>
-      <c r="H43" s="138"/>
+      <c r="G43" s="156"/>
+      <c r="H43" s="129"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="20"/>
-      <c r="B44" s="139" t="s">
+      <c r="B44" s="124" t="s">
         <v>2407</v>
       </c>
-      <c r="C44" s="137" t="s">
+      <c r="C44" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="137" t="s">
+      <c r="D44" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="137" t="s">
+      <c r="E44" s="127" t="s">
         <v>40</v>
       </c>
       <c r="F44" s="4">
         <v>25.6</v>
       </c>
-      <c r="G44" s="153">
+      <c r="G44" s="155">
         <v>0.28399999999999997</v>
       </c>
       <c r="H44" s="4" t="s">
@@ -33511,60 +33511,60 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="20"/>
-      <c r="B45" s="140"/>
-      <c r="C45" s="142"/>
-      <c r="D45" s="142"/>
-      <c r="E45" s="142"/>
+      <c r="B45" s="125"/>
+      <c r="C45" s="128"/>
+      <c r="D45" s="128"/>
+      <c r="E45" s="128"/>
       <c r="F45" s="4" t="s">
         <v>2405</v>
       </c>
-      <c r="G45" s="155"/>
+      <c r="G45" s="162"/>
       <c r="H45" s="4" t="s">
         <v>2409</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="20"/>
-      <c r="B46" s="140"/>
-      <c r="C46" s="142"/>
-      <c r="D46" s="142"/>
-      <c r="E46" s="142"/>
+      <c r="B46" s="125"/>
+      <c r="C46" s="128"/>
+      <c r="D46" s="128"/>
+      <c r="E46" s="128"/>
       <c r="F46" s="11"/>
-      <c r="G46" s="155"/>
+      <c r="G46" s="162"/>
       <c r="H46" s="4" t="s">
         <v>2410</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="23" thickBot="1">
       <c r="A47" s="20"/>
-      <c r="B47" s="141"/>
-      <c r="C47" s="138"/>
-      <c r="D47" s="138"/>
-      <c r="E47" s="138"/>
+      <c r="B47" s="126"/>
+      <c r="C47" s="129"/>
+      <c r="D47" s="129"/>
+      <c r="E47" s="129"/>
       <c r="F47" s="12"/>
-      <c r="G47" s="154"/>
+      <c r="G47" s="156"/>
       <c r="H47" s="2" t="s">
         <v>2411</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="20"/>
-      <c r="B48" s="139" t="s">
+      <c r="B48" s="124" t="s">
         <v>2412</v>
       </c>
-      <c r="C48" s="137" t="s">
+      <c r="C48" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="D48" s="137" t="s">
+      <c r="D48" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="E48" s="137" t="s">
+      <c r="E48" s="127" t="s">
         <v>40</v>
       </c>
       <c r="F48" s="4">
         <v>30.9</v>
       </c>
-      <c r="G48" s="162">
+      <c r="G48" s="152">
         <v>0.3</v>
       </c>
       <c r="H48" s="4" t="s">
@@ -33572,14 +33572,14 @@
       </c>
     </row>
     <row r="49" spans="2:10" s="21" customFormat="1">
-      <c r="B49" s="140"/>
-      <c r="C49" s="142"/>
-      <c r="D49" s="142"/>
-      <c r="E49" s="142"/>
+      <c r="B49" s="125"/>
+      <c r="C49" s="128"/>
+      <c r="D49" s="128"/>
+      <c r="E49" s="128"/>
       <c r="F49" s="4" t="s">
         <v>2405</v>
       </c>
-      <c r="G49" s="163"/>
+      <c r="G49" s="153"/>
       <c r="H49" s="4" t="s">
         <v>2414</v>
       </c>
@@ -33587,78 +33587,78 @@
       <c r="J49"/>
     </row>
     <row r="50" spans="2:10">
-      <c r="B50" s="140"/>
-      <c r="C50" s="142"/>
-      <c r="D50" s="142"/>
-      <c r="E50" s="142"/>
+      <c r="B50" s="125"/>
+      <c r="C50" s="128"/>
+      <c r="D50" s="128"/>
+      <c r="E50" s="128"/>
       <c r="F50" s="11"/>
-      <c r="G50" s="163"/>
+      <c r="G50" s="153"/>
       <c r="H50" s="4" t="s">
         <v>2415</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="23" thickBot="1">
-      <c r="B51" s="141"/>
-      <c r="C51" s="138"/>
-      <c r="D51" s="138"/>
-      <c r="E51" s="138"/>
+      <c r="B51" s="126"/>
+      <c r="C51" s="129"/>
+      <c r="D51" s="129"/>
+      <c r="E51" s="129"/>
       <c r="F51" s="12"/>
-      <c r="G51" s="164"/>
+      <c r="G51" s="154"/>
       <c r="H51" s="2" t="s">
         <v>2411</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="28" customHeight="1">
-      <c r="B52" s="139" t="s">
+      <c r="B52" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="137" t="s">
+      <c r="C52" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="D52" s="137" t="s">
+      <c r="D52" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="E52" s="137" t="s">
+      <c r="E52" s="127" t="s">
         <v>40</v>
       </c>
       <c r="F52" s="4">
         <v>63.1</v>
       </c>
-      <c r="G52" s="153">
+      <c r="G52" s="155">
         <v>0.59499999999999997</v>
       </c>
-      <c r="H52" s="137" t="s">
+      <c r="H52" s="127" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="16" thickBot="1">
-      <c r="B53" s="141"/>
-      <c r="C53" s="138"/>
-      <c r="D53" s="138"/>
-      <c r="E53" s="138"/>
+      <c r="B53" s="126"/>
+      <c r="C53" s="129"/>
+      <c r="D53" s="129"/>
+      <c r="E53" s="129"/>
       <c r="F53" s="2" t="s">
         <v>2405</v>
       </c>
-      <c r="G53" s="154"/>
-      <c r="H53" s="138"/>
+      <c r="G53" s="156"/>
+      <c r="H53" s="129"/>
     </row>
     <row r="54" spans="2:10">
-      <c r="B54" s="139" t="s">
+      <c r="B54" s="124" t="s">
         <v>2416</v>
       </c>
-      <c r="C54" s="137" t="s">
+      <c r="C54" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="D54" s="137" t="s">
+      <c r="D54" s="127" t="s">
         <v>2417</v>
       </c>
-      <c r="E54" s="137" t="s">
+      <c r="E54" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="F54" s="137" t="s">
+      <c r="F54" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="G54" s="137" t="s">
+      <c r="G54" s="127" t="s">
         <v>24</v>
       </c>
       <c r="H54" s="4" t="s">
@@ -33666,70 +33666,70 @@
       </c>
     </row>
     <row r="55" spans="2:10">
-      <c r="B55" s="140"/>
-      <c r="C55" s="142"/>
-      <c r="D55" s="142"/>
-      <c r="E55" s="142"/>
-      <c r="F55" s="142"/>
-      <c r="G55" s="142"/>
+      <c r="B55" s="125"/>
+      <c r="C55" s="128"/>
+      <c r="D55" s="128"/>
+      <c r="E55" s="128"/>
+      <c r="F55" s="128"/>
+      <c r="G55" s="128"/>
       <c r="H55" s="4" t="s">
         <v>2419</v>
       </c>
     </row>
     <row r="56" spans="2:10">
-      <c r="B56" s="140"/>
-      <c r="C56" s="142"/>
-      <c r="D56" s="142"/>
-      <c r="E56" s="142"/>
-      <c r="F56" s="142"/>
-      <c r="G56" s="142"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="128"/>
+      <c r="D56" s="128"/>
+      <c r="E56" s="128"/>
+      <c r="F56" s="128"/>
+      <c r="G56" s="128"/>
       <c r="H56" s="4" t="s">
         <v>2420</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="16" thickBot="1">
-      <c r="B57" s="141"/>
-      <c r="C57" s="138"/>
-      <c r="D57" s="138"/>
-      <c r="E57" s="138"/>
-      <c r="F57" s="138"/>
-      <c r="G57" s="138"/>
+      <c r="B57" s="126"/>
+      <c r="C57" s="129"/>
+      <c r="D57" s="129"/>
+      <c r="E57" s="129"/>
+      <c r="F57" s="129"/>
+      <c r="G57" s="129"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="2:10">
-      <c r="B58" s="120"/>
-      <c r="C58" s="121"/>
-      <c r="D58" s="121"/>
-      <c r="E58" s="121"/>
-      <c r="F58" s="121"/>
-      <c r="G58" s="121"/>
-      <c r="H58" s="122"/>
+      <c r="B58" s="143"/>
+      <c r="C58" s="144"/>
+      <c r="D58" s="144"/>
+      <c r="E58" s="144"/>
+      <c r="F58" s="144"/>
+      <c r="G58" s="144"/>
+      <c r="H58" s="145"/>
     </row>
     <row r="59" spans="2:10">
-      <c r="B59" s="123" t="s">
+      <c r="B59" s="146" t="s">
         <v>43</v>
       </c>
-      <c r="C59" s="124"/>
-      <c r="D59" s="124"/>
-      <c r="E59" s="124"/>
-      <c r="F59" s="124"/>
-      <c r="G59" s="124"/>
-      <c r="H59" s="125"/>
+      <c r="C59" s="147"/>
+      <c r="D59" s="147"/>
+      <c r="E59" s="147"/>
+      <c r="F59" s="147"/>
+      <c r="G59" s="147"/>
+      <c r="H59" s="148"/>
     </row>
     <row r="60" spans="2:10" ht="16" thickBot="1">
-      <c r="B60" s="126"/>
-      <c r="C60" s="127"/>
-      <c r="D60" s="127"/>
-      <c r="E60" s="127"/>
-      <c r="F60" s="127"/>
-      <c r="G60" s="127"/>
-      <c r="H60" s="128"/>
+      <c r="B60" s="149"/>
+      <c r="C60" s="150"/>
+      <c r="D60" s="150"/>
+      <c r="E60" s="150"/>
+      <c r="F60" s="150"/>
+      <c r="G60" s="150"/>
+      <c r="H60" s="151"/>
     </row>
     <row r="61" spans="2:10" ht="45">
-      <c r="B61" s="139" t="s">
+      <c r="B61" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="C61" s="137" t="s">
+      <c r="C61" s="127" t="s">
         <v>45</v>
       </c>
       <c r="D61" s="5" t="s">
@@ -33738,58 +33738,58 @@
       <c r="E61" s="4">
         <v>4.88</v>
       </c>
-      <c r="F61" s="137" t="s">
+      <c r="F61" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="G61" s="137" t="s">
+      <c r="G61" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H61" s="137" t="s">
+      <c r="H61" s="127" t="s">
         <v>2424</v>
       </c>
     </row>
     <row r="62" spans="2:10">
-      <c r="B62" s="140"/>
-      <c r="C62" s="142"/>
+      <c r="B62" s="125"/>
+      <c r="C62" s="128"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
         <v>2423</v>
       </c>
-      <c r="F62" s="142"/>
-      <c r="G62" s="142"/>
-      <c r="H62" s="142"/>
+      <c r="F62" s="128"/>
+      <c r="G62" s="128"/>
+      <c r="H62" s="128"/>
     </row>
     <row r="63" spans="2:10" ht="31" thickBot="1">
-      <c r="B63" s="141"/>
-      <c r="C63" s="138"/>
+      <c r="B63" s="126"/>
+      <c r="C63" s="129"/>
       <c r="D63" s="13" t="s">
         <v>2422</v>
       </c>
       <c r="E63" s="12"/>
-      <c r="F63" s="138"/>
-      <c r="G63" s="138"/>
-      <c r="H63" s="138"/>
+      <c r="F63" s="129"/>
+      <c r="G63" s="129"/>
+      <c r="H63" s="129"/>
     </row>
     <row r="64" spans="2:10" ht="45">
       <c r="B64" s="3" t="s">
         <v>2425</v>
       </c>
-      <c r="C64" s="137" t="s">
+      <c r="C64" s="127" t="s">
         <v>45</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>2427</v>
       </c>
-      <c r="E64" s="153">
+      <c r="E64" s="155">
         <v>2.3E-2</v>
       </c>
-      <c r="F64" s="153">
+      <c r="F64" s="155">
         <v>2.3E-2</v>
       </c>
-      <c r="G64" s="153">
+      <c r="G64" s="155">
         <v>2.3E-2</v>
       </c>
-      <c r="H64" s="137" t="s">
+      <c r="H64" s="127" t="s">
         <v>2428</v>
       </c>
     </row>
@@ -33797,17 +33797,17 @@
       <c r="B65" s="1" t="s">
         <v>2426</v>
       </c>
-      <c r="C65" s="138"/>
+      <c r="C65" s="129"/>
       <c r="D65" s="13" t="s">
         <v>2422</v>
       </c>
-      <c r="E65" s="154"/>
-      <c r="F65" s="154"/>
-      <c r="G65" s="154"/>
-      <c r="H65" s="138"/>
+      <c r="E65" s="156"/>
+      <c r="F65" s="156"/>
+      <c r="G65" s="156"/>
+      <c r="H65" s="129"/>
     </row>
     <row r="66" spans="2:8" ht="45">
-      <c r="B66" s="139" t="s">
+      <c r="B66" s="124" t="s">
         <v>46</v>
       </c>
       <c r="C66" s="4" t="s">
@@ -33819,10 +33819,10 @@
       <c r="E66" s="110">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F66" s="137" t="s">
+      <c r="F66" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="G66" s="137" t="s">
+      <c r="G66" s="127" t="s">
         <v>24</v>
       </c>
       <c r="H66" s="4" t="s">
@@ -33830,7 +33830,7 @@
       </c>
     </row>
     <row r="67" spans="2:8" ht="22">
-      <c r="B67" s="140"/>
+      <c r="B67" s="125"/>
       <c r="C67" s="4" t="s">
         <v>2429</v>
       </c>
@@ -33838,14 +33838,14 @@
       <c r="E67" s="4" t="s">
         <v>2433</v>
       </c>
-      <c r="F67" s="142"/>
-      <c r="G67" s="142"/>
+      <c r="F67" s="128"/>
+      <c r="G67" s="128"/>
       <c r="H67" s="4" t="s">
         <v>2435</v>
       </c>
     </row>
     <row r="68" spans="2:8">
-      <c r="B68" s="140"/>
+      <c r="B68" s="125"/>
       <c r="C68" s="4" t="s">
         <v>2430</v>
       </c>
@@ -33853,32 +33853,32 @@
         <v>4</v>
       </c>
       <c r="E68" s="11"/>
-      <c r="F68" s="142"/>
-      <c r="G68" s="142"/>
+      <c r="F68" s="128"/>
+      <c r="G68" s="128"/>
       <c r="H68" s="11"/>
     </row>
     <row r="69" spans="2:8">
-      <c r="B69" s="140"/>
+      <c r="B69" s="125"/>
       <c r="C69" s="4"/>
       <c r="D69" s="5" t="s">
         <v>2432</v>
       </c>
       <c r="E69" s="11"/>
-      <c r="F69" s="142"/>
-      <c r="G69" s="142"/>
+      <c r="F69" s="128"/>
+      <c r="G69" s="128"/>
       <c r="H69" s="11"/>
     </row>
     <row r="70" spans="2:8" ht="16" thickBot="1">
-      <c r="B70" s="141"/>
+      <c r="B70" s="126"/>
       <c r="C70" s="12"/>
       <c r="D70" s="2"/>
       <c r="E70" s="12"/>
-      <c r="F70" s="138"/>
-      <c r="G70" s="138"/>
+      <c r="F70" s="129"/>
+      <c r="G70" s="129"/>
       <c r="H70" s="12"/>
     </row>
     <row r="71" spans="2:8" ht="45">
-      <c r="B71" s="139" t="s">
+      <c r="B71" s="124" t="s">
         <v>47</v>
       </c>
       <c r="C71" s="4" t="s">
@@ -33890,10 +33890,10 @@
       <c r="E71" s="110">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F71" s="137" t="s">
+      <c r="F71" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="G71" s="137" t="s">
+      <c r="G71" s="127" t="s">
         <v>24</v>
       </c>
       <c r="H71" s="4" t="s">
@@ -33901,7 +33901,7 @@
       </c>
     </row>
     <row r="72" spans="2:8" ht="22">
-      <c r="B72" s="140"/>
+      <c r="B72" s="125"/>
       <c r="C72" s="4" t="s">
         <v>48</v>
       </c>
@@ -33909,38 +33909,38 @@
       <c r="E72" s="4" t="s">
         <v>2433</v>
       </c>
-      <c r="F72" s="142"/>
-      <c r="G72" s="142"/>
+      <c r="F72" s="128"/>
+      <c r="G72" s="128"/>
       <c r="H72" s="4" t="s">
         <v>2439</v>
       </c>
     </row>
     <row r="73" spans="2:8" ht="22">
-      <c r="B73" s="140"/>
+      <c r="B73" s="125"/>
       <c r="C73" s="4"/>
       <c r="D73" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E73" s="11"/>
-      <c r="F73" s="142"/>
-      <c r="G73" s="142"/>
+      <c r="F73" s="128"/>
+      <c r="G73" s="128"/>
       <c r="H73" s="4" t="s">
         <v>2440</v>
       </c>
     </row>
     <row r="74" spans="2:8" ht="16" thickBot="1">
-      <c r="B74" s="141"/>
+      <c r="B74" s="126"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13" t="s">
         <v>2437</v>
       </c>
       <c r="E74" s="12"/>
-      <c r="F74" s="138"/>
-      <c r="G74" s="138"/>
+      <c r="F74" s="129"/>
+      <c r="G74" s="129"/>
       <c r="H74" s="2"/>
     </row>
     <row r="75" spans="2:8" ht="44">
-      <c r="B75" s="129" t="s">
+      <c r="B75" s="136" t="s">
         <v>2441</v>
       </c>
       <c r="C75" s="6" t="s">
@@ -33949,13 +33949,13 @@
       <c r="D75" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E75" s="135" t="s">
+      <c r="E75" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="F75" s="135" t="s">
+      <c r="F75" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="G75" s="135" t="s">
+      <c r="G75" s="130" t="s">
         <v>24</v>
       </c>
       <c r="H75" s="6" t="s">
@@ -33963,67 +33963,67 @@
       </c>
     </row>
     <row r="76" spans="2:8" ht="44">
-      <c r="B76" s="146"/>
+      <c r="B76" s="137"/>
       <c r="C76" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>2442</v>
       </c>
-      <c r="E76" s="147"/>
-      <c r="F76" s="147"/>
-      <c r="G76" s="147"/>
+      <c r="E76" s="139"/>
+      <c r="F76" s="139"/>
+      <c r="G76" s="139"/>
       <c r="H76" s="6" t="s">
         <v>2444</v>
       </c>
     </row>
     <row r="77" spans="2:8" ht="34" thickBot="1">
-      <c r="B77" s="130"/>
+      <c r="B77" s="138"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
-      <c r="E77" s="136"/>
-      <c r="F77" s="136"/>
-      <c r="G77" s="136"/>
+      <c r="E77" s="131"/>
+      <c r="F77" s="131"/>
+      <c r="G77" s="131"/>
       <c r="H77" s="10" t="s">
         <v>2445</v>
       </c>
     </row>
     <row r="78" spans="2:8">
-      <c r="B78" s="139" t="s">
+      <c r="B78" s="124" t="s">
         <v>50</v>
       </c>
-      <c r="C78" s="137" t="s">
+      <c r="C78" s="127" t="s">
         <v>45</v>
       </c>
-      <c r="D78" s="137" t="s">
+      <c r="D78" s="127" t="s">
         <v>2446</v>
       </c>
-      <c r="E78" s="137" t="s">
+      <c r="E78" s="127" t="s">
         <v>24</v>
       </c>
       <c r="F78" s="4">
         <v>11.2</v>
       </c>
-      <c r="G78" s="137" t="s">
+      <c r="G78" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H78" s="137" t="s">
+      <c r="H78" s="127" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="79" spans="2:8" ht="16" thickBot="1">
-      <c r="B79" s="141"/>
-      <c r="C79" s="138"/>
-      <c r="D79" s="138"/>
-      <c r="E79" s="138"/>
+      <c r="B79" s="126"/>
+      <c r="C79" s="129"/>
+      <c r="D79" s="129"/>
+      <c r="E79" s="129"/>
       <c r="F79" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G79" s="138"/>
-      <c r="H79" s="138"/>
+      <c r="G79" s="129"/>
+      <c r="H79" s="129"/>
     </row>
     <row r="80" spans="2:8" ht="30">
-      <c r="B80" s="139" t="s">
+      <c r="B80" s="124" t="s">
         <v>52</v>
       </c>
       <c r="C80" s="4" t="s">
@@ -34046,7 +34046,7 @@
       </c>
     </row>
     <row r="81" spans="2:8" ht="44">
-      <c r="B81" s="140"/>
+      <c r="B81" s="125"/>
       <c r="C81" s="4" t="s">
         <v>54</v>
       </c>
@@ -34065,7 +34065,7 @@
       </c>
     </row>
     <row r="82" spans="2:8" ht="45">
-      <c r="B82" s="140"/>
+      <c r="B82" s="125"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4" t="s">
@@ -34080,7 +34080,7 @@
       </c>
     </row>
     <row r="83" spans="2:8" ht="30">
-      <c r="B83" s="140"/>
+      <c r="B83" s="125"/>
       <c r="C83" s="5" t="s">
         <v>55</v>
       </c>
@@ -34099,7 +34099,7 @@
       </c>
     </row>
     <row r="84" spans="2:8" ht="22">
-      <c r="B84" s="140"/>
+      <c r="B84" s="125"/>
       <c r="C84" s="11"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
@@ -34114,7 +34114,7 @@
       </c>
     </row>
     <row r="85" spans="2:8">
-      <c r="B85" s="140"/>
+      <c r="B85" s="125"/>
       <c r="C85" s="11"/>
       <c r="D85" s="5" t="s">
         <v>4</v>
@@ -34125,7 +34125,7 @@
       <c r="H85" s="4"/>
     </row>
     <row r="86" spans="2:8">
-      <c r="B86" s="140"/>
+      <c r="B86" s="125"/>
       <c r="C86" s="11"/>
       <c r="D86" s="5" t="s">
         <v>58</v>
@@ -34136,7 +34136,7 @@
       <c r="H86" s="11"/>
     </row>
     <row r="87" spans="2:8" ht="16" thickBot="1">
-      <c r="B87" s="141"/>
+      <c r="B87" s="126"/>
       <c r="C87" s="12"/>
       <c r="D87" s="2"/>
       <c r="E87" s="12"/>
@@ -34145,36 +34145,36 @@
       <c r="H87" s="12"/>
     </row>
     <row r="88" spans="2:8">
-      <c r="B88" s="120"/>
-      <c r="C88" s="121"/>
-      <c r="D88" s="121"/>
-      <c r="E88" s="121"/>
-      <c r="F88" s="121"/>
-      <c r="G88" s="121"/>
-      <c r="H88" s="122"/>
+      <c r="B88" s="143"/>
+      <c r="C88" s="144"/>
+      <c r="D88" s="144"/>
+      <c r="E88" s="144"/>
+      <c r="F88" s="144"/>
+      <c r="G88" s="144"/>
+      <c r="H88" s="145"/>
     </row>
     <row r="89" spans="2:8">
-      <c r="B89" s="123" t="s">
+      <c r="B89" s="146" t="s">
         <v>74</v>
       </c>
-      <c r="C89" s="124"/>
-      <c r="D89" s="124"/>
-      <c r="E89" s="124"/>
-      <c r="F89" s="124"/>
-      <c r="G89" s="124"/>
-      <c r="H89" s="125"/>
+      <c r="C89" s="147"/>
+      <c r="D89" s="147"/>
+      <c r="E89" s="147"/>
+      <c r="F89" s="147"/>
+      <c r="G89" s="147"/>
+      <c r="H89" s="148"/>
     </row>
     <row r="90" spans="2:8" ht="16" thickBot="1">
-      <c r="B90" s="126"/>
-      <c r="C90" s="127"/>
-      <c r="D90" s="127"/>
-      <c r="E90" s="127"/>
-      <c r="F90" s="127"/>
-      <c r="G90" s="127"/>
-      <c r="H90" s="128"/>
+      <c r="B90" s="149"/>
+      <c r="C90" s="150"/>
+      <c r="D90" s="150"/>
+      <c r="E90" s="150"/>
+      <c r="F90" s="150"/>
+      <c r="G90" s="150"/>
+      <c r="H90" s="151"/>
     </row>
     <row r="91" spans="2:8" ht="30">
-      <c r="B91" s="129" t="s">
+      <c r="B91" s="136" t="s">
         <v>75</v>
       </c>
       <c r="C91" s="6" t="s">
@@ -34192,12 +34192,12 @@
       <c r="G91" s="6">
         <v>2.9</v>
       </c>
-      <c r="H91" s="135" t="s">
+      <c r="H91" s="130" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="92" spans="2:8" ht="60">
-      <c r="B92" s="146"/>
+      <c r="B92" s="137"/>
       <c r="C92" s="9" t="s">
         <v>76</v>
       </c>
@@ -34211,10 +34211,10 @@
       <c r="G92" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H92" s="147"/>
+      <c r="H92" s="139"/>
     </row>
     <row r="93" spans="2:8" ht="75">
-      <c r="B93" s="146"/>
+      <c r="B93" s="137"/>
       <c r="C93" s="9" t="s">
         <v>77</v>
       </c>
@@ -34224,10 +34224,10 @@
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
-      <c r="H93" s="147"/>
+      <c r="H93" s="139"/>
     </row>
     <row r="94" spans="2:8" ht="31" thickBot="1">
-      <c r="B94" s="130"/>
+      <c r="B94" s="138"/>
       <c r="C94" s="10"/>
       <c r="D94" s="14" t="s">
         <v>80</v>
@@ -34235,25 +34235,25 @@
       <c r="E94" s="8"/>
       <c r="F94" s="8"/>
       <c r="G94" s="8"/>
-      <c r="H94" s="136"/>
+      <c r="H94" s="131"/>
     </row>
     <row r="95" spans="2:8">
-      <c r="B95" s="139" t="s">
+      <c r="B95" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="C95" s="137" t="s">
+      <c r="C95" s="127" t="s">
         <v>53</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E95" s="137" t="s">
+      <c r="E95" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="F95" s="137" t="s">
+      <c r="F95" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="G95" s="137">
+      <c r="G95" s="127">
         <v>92.2</v>
       </c>
       <c r="H95" s="4" t="s">
@@ -34261,113 +34261,113 @@
       </c>
     </row>
     <row r="96" spans="2:8">
-      <c r="B96" s="140"/>
-      <c r="C96" s="142"/>
+      <c r="B96" s="125"/>
+      <c r="C96" s="128"/>
       <c r="D96" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E96" s="142"/>
-      <c r="F96" s="142"/>
-      <c r="G96" s="142"/>
+      <c r="E96" s="128"/>
+      <c r="F96" s="128"/>
+      <c r="G96" s="128"/>
       <c r="H96" s="4"/>
     </row>
     <row r="97" spans="2:8" ht="44">
-      <c r="B97" s="140"/>
-      <c r="C97" s="142"/>
+      <c r="B97" s="125"/>
+      <c r="C97" s="128"/>
       <c r="D97" s="4"/>
-      <c r="E97" s="142"/>
-      <c r="F97" s="142"/>
-      <c r="G97" s="142"/>
+      <c r="E97" s="128"/>
+      <c r="F97" s="128"/>
+      <c r="G97" s="128"/>
       <c r="H97" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="98" spans="2:8">
-      <c r="B98" s="140"/>
-      <c r="C98" s="142"/>
+      <c r="B98" s="125"/>
+      <c r="C98" s="128"/>
       <c r="D98" s="11"/>
-      <c r="E98" s="142"/>
-      <c r="F98" s="142"/>
-      <c r="G98" s="142"/>
+      <c r="E98" s="128"/>
+      <c r="F98" s="128"/>
+      <c r="G98" s="128"/>
       <c r="H98" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="99" spans="2:8">
-      <c r="B99" s="140"/>
-      <c r="C99" s="142"/>
+      <c r="B99" s="125"/>
+      <c r="C99" s="128"/>
       <c r="D99" s="11"/>
-      <c r="E99" s="142"/>
-      <c r="F99" s="142"/>
-      <c r="G99" s="142"/>
+      <c r="E99" s="128"/>
+      <c r="F99" s="128"/>
+      <c r="G99" s="128"/>
       <c r="H99" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="100" spans="2:8">
-      <c r="B100" s="140"/>
-      <c r="C100" s="142"/>
+      <c r="B100" s="125"/>
+      <c r="C100" s="128"/>
       <c r="D100" s="11"/>
-      <c r="E100" s="142"/>
-      <c r="F100" s="142"/>
-      <c r="G100" s="142"/>
+      <c r="E100" s="128"/>
+      <c r="F100" s="128"/>
+      <c r="G100" s="128"/>
       <c r="H100" s="4"/>
     </row>
     <row r="101" spans="2:8" ht="33">
-      <c r="B101" s="140"/>
-      <c r="C101" s="142"/>
+      <c r="B101" s="125"/>
+      <c r="C101" s="128"/>
       <c r="D101" s="11"/>
-      <c r="E101" s="142"/>
-      <c r="F101" s="142"/>
-      <c r="G101" s="142"/>
+      <c r="E101" s="128"/>
+      <c r="F101" s="128"/>
+      <c r="G101" s="128"/>
       <c r="H101" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="102" spans="2:8">
-      <c r="B102" s="140"/>
-      <c r="C102" s="142"/>
+      <c r="B102" s="125"/>
+      <c r="C102" s="128"/>
       <c r="D102" s="11"/>
-      <c r="E102" s="142"/>
-      <c r="F102" s="142"/>
-      <c r="G102" s="142"/>
+      <c r="E102" s="128"/>
+      <c r="F102" s="128"/>
+      <c r="G102" s="128"/>
       <c r="H102" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="103" spans="2:8">
-      <c r="B103" s="140"/>
-      <c r="C103" s="142"/>
+      <c r="B103" s="125"/>
+      <c r="C103" s="128"/>
       <c r="D103" s="11"/>
-      <c r="E103" s="142"/>
-      <c r="F103" s="142"/>
-      <c r="G103" s="142"/>
+      <c r="E103" s="128"/>
+      <c r="F103" s="128"/>
+      <c r="G103" s="128"/>
       <c r="H103" s="4"/>
     </row>
     <row r="104" spans="2:8" ht="33">
-      <c r="B104" s="140"/>
-      <c r="C104" s="142"/>
+      <c r="B104" s="125"/>
+      <c r="C104" s="128"/>
       <c r="D104" s="11"/>
-      <c r="E104" s="142"/>
-      <c r="F104" s="142"/>
-      <c r="G104" s="142"/>
+      <c r="E104" s="128"/>
+      <c r="F104" s="128"/>
+      <c r="G104" s="128"/>
       <c r="H104" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="105" spans="2:8" ht="16" thickBot="1">
-      <c r="B105" s="141"/>
-      <c r="C105" s="138"/>
+      <c r="B105" s="126"/>
+      <c r="C105" s="129"/>
       <c r="D105" s="12"/>
-      <c r="E105" s="138"/>
-      <c r="F105" s="138"/>
-      <c r="G105" s="138"/>
+      <c r="E105" s="129"/>
+      <c r="F105" s="129"/>
+      <c r="G105" s="129"/>
       <c r="H105" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="106" spans="2:8">
-      <c r="B106" s="139" t="s">
+      <c r="B106" s="124" t="s">
         <v>94</v>
       </c>
       <c r="C106" s="4" t="s">
@@ -34390,7 +34390,7 @@
       </c>
     </row>
     <row r="107" spans="2:8" ht="33">
-      <c r="B107" s="140"/>
+      <c r="B107" s="125"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4" t="s">
         <v>98</v>
@@ -34409,7 +34409,7 @@
       </c>
     </row>
     <row r="108" spans="2:8" ht="110">
-      <c r="B108" s="140"/>
+      <c r="B108" s="125"/>
       <c r="C108" s="4" t="s">
         <v>96</v>
       </c>
@@ -34420,7 +34420,7 @@
       <c r="H108" s="4"/>
     </row>
     <row r="109" spans="2:8">
-      <c r="B109" s="140"/>
+      <c r="B109" s="125"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4" t="s">
         <v>99</v>
@@ -34431,7 +34431,7 @@
       <c r="H109" s="11"/>
     </row>
     <row r="110" spans="2:8">
-      <c r="B110" s="140"/>
+      <c r="B110" s="125"/>
       <c r="C110" s="11"/>
       <c r="D110" s="5" t="s">
         <v>4</v>
@@ -34442,7 +34442,7 @@
       <c r="H110" s="11"/>
     </row>
     <row r="111" spans="2:8">
-      <c r="B111" s="140"/>
+      <c r="B111" s="125"/>
       <c r="C111" s="11"/>
       <c r="D111" s="5" t="s">
         <v>100</v>
@@ -34453,7 +34453,7 @@
       <c r="H111" s="11"/>
     </row>
     <row r="112" spans="2:8">
-      <c r="B112" s="140"/>
+      <c r="B112" s="125"/>
       <c r="C112" s="11"/>
       <c r="D112" s="4"/>
       <c r="E112" s="11"/>
@@ -34462,7 +34462,7 @@
       <c r="H112" s="11"/>
     </row>
     <row r="113" spans="1:8" ht="16" thickBot="1">
-      <c r="B113" s="141"/>
+      <c r="B113" s="126"/>
       <c r="C113" s="12"/>
       <c r="D113" s="2"/>
       <c r="E113" s="12"/>
@@ -34471,7 +34471,7 @@
       <c r="H113" s="12"/>
     </row>
     <row r="114" spans="1:8">
-      <c r="B114" s="139" t="s">
+      <c r="B114" s="124" t="s">
         <v>105</v>
       </c>
       <c r="C114" s="4" t="s">
@@ -34494,7 +34494,7 @@
       </c>
     </row>
     <row r="115" spans="1:8" ht="22">
-      <c r="B115" s="140"/>
+      <c r="B115" s="125"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4" t="s">
         <v>107</v>
@@ -34511,7 +34511,7 @@
       </c>
     </row>
     <row r="116" spans="1:8">
-      <c r="B116" s="140"/>
+      <c r="B116" s="125"/>
       <c r="C116" s="4" t="s">
         <v>106</v>
       </c>
@@ -34524,7 +34524,7 @@
       <c r="H116" s="11"/>
     </row>
     <row r="117" spans="1:8" ht="16" thickBot="1">
-      <c r="B117" s="141"/>
+      <c r="B117" s="126"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13" t="s">
         <v>108</v>
@@ -34539,7 +34539,7 @@
       <c r="H117" s="12"/>
     </row>
     <row r="118" spans="1:8">
-      <c r="B118" s="129" t="s">
+      <c r="B118" s="136" t="s">
         <v>110</v>
       </c>
       <c r="C118" s="6" t="s">
@@ -34548,10 +34548,10 @@
       <c r="D118" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E118" s="135">
+      <c r="E118" s="130">
         <v>96</v>
       </c>
-      <c r="F118" s="135">
+      <c r="F118" s="130">
         <v>92</v>
       </c>
       <c r="G118" s="6" t="s">
@@ -34562,13 +34562,13 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="33">
-      <c r="B119" s="146"/>
+      <c r="B119" s="137"/>
       <c r="C119" s="6"/>
       <c r="D119" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E119" s="147"/>
-      <c r="F119" s="147"/>
+      <c r="E119" s="139"/>
+      <c r="F119" s="139"/>
       <c r="G119" s="6" t="s">
         <v>9</v>
       </c>
@@ -34577,75 +34577,75 @@
       </c>
     </row>
     <row r="120" spans="1:8" ht="55">
-      <c r="B120" s="146"/>
+      <c r="B120" s="137"/>
       <c r="C120" s="6" t="s">
         <v>112</v>
       </c>
       <c r="D120" s="6"/>
-      <c r="E120" s="147"/>
-      <c r="F120" s="147"/>
+      <c r="E120" s="139"/>
+      <c r="F120" s="139"/>
       <c r="G120" s="6" t="s">
         <v>117</v>
       </c>
       <c r="H120" s="6"/>
     </row>
     <row r="121" spans="1:8">
-      <c r="B121" s="146"/>
+      <c r="B121" s="137"/>
       <c r="C121" s="6"/>
       <c r="D121" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E121" s="147"/>
-      <c r="F121" s="147"/>
+      <c r="E121" s="139"/>
+      <c r="F121" s="139"/>
       <c r="G121" s="6" t="s">
         <v>118</v>
       </c>
       <c r="H121" s="7"/>
     </row>
     <row r="122" spans="1:8" ht="55">
-      <c r="B122" s="146"/>
+      <c r="B122" s="137"/>
       <c r="C122" s="6" t="s">
         <v>113</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E122" s="147"/>
-      <c r="F122" s="147"/>
+      <c r="E122" s="139"/>
+      <c r="F122" s="139"/>
       <c r="G122" s="6" t="s">
         <v>119</v>
       </c>
       <c r="H122" s="7"/>
     </row>
     <row r="123" spans="1:8" ht="22">
-      <c r="B123" s="146"/>
+      <c r="B123" s="137"/>
       <c r="C123" s="6"/>
       <c r="D123" s="7"/>
-      <c r="E123" s="147"/>
-      <c r="F123" s="147"/>
+      <c r="E123" s="139"/>
+      <c r="F123" s="139"/>
       <c r="G123" s="6" t="s">
         <v>120</v>
       </c>
       <c r="H123" s="7"/>
     </row>
     <row r="124" spans="1:8" ht="16" thickBot="1">
-      <c r="B124" s="130"/>
+      <c r="B124" s="138"/>
       <c r="C124" s="10"/>
       <c r="D124" s="8"/>
-      <c r="E124" s="136"/>
-      <c r="F124" s="136"/>
+      <c r="E124" s="131"/>
+      <c r="F124" s="131"/>
       <c r="G124" s="8"/>
       <c r="H124" s="8"/>
     </row>
     <row r="125" spans="1:8">
       <c r="A125" s="20"/>
-      <c r="B125" s="139" t="s">
+      <c r="B125" s="124" t="s">
         <v>122</v>
       </c>
-      <c r="C125" s="137" t="s">
+      <c r="C125" s="127" t="s">
         <v>123</v>
       </c>
-      <c r="D125" s="137" t="s">
+      <c r="D125" s="127" t="s">
         <v>124</v>
       </c>
       <c r="E125" s="4">
@@ -34654,44 +34654,44 @@
       <c r="F125" s="4">
         <v>70</v>
       </c>
-      <c r="G125" s="137" t="s">
+      <c r="G125" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H125" s="137" t="s">
+      <c r="H125" s="127" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="126" spans="1:8">
       <c r="A126" s="20"/>
-      <c r="B126" s="140"/>
-      <c r="C126" s="142"/>
-      <c r="D126" s="142"/>
+      <c r="B126" s="125"/>
+      <c r="C126" s="128"/>
+      <c r="D126" s="128"/>
       <c r="E126" s="4" t="s">
         <v>101</v>
       </c>
       <c r="F126" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G126" s="142"/>
-      <c r="H126" s="142"/>
+      <c r="G126" s="128"/>
+      <c r="H126" s="128"/>
     </row>
     <row r="127" spans="1:8" ht="23" thickBot="1">
       <c r="A127" s="20"/>
-      <c r="B127" s="141"/>
-      <c r="C127" s="138"/>
-      <c r="D127" s="138"/>
+      <c r="B127" s="126"/>
+      <c r="C127" s="129"/>
+      <c r="D127" s="129"/>
       <c r="E127" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F127" s="12"/>
-      <c r="G127" s="138"/>
-      <c r="H127" s="138"/>
+      <c r="G127" s="129"/>
+      <c r="H127" s="129"/>
     </row>
     <row r="128" spans="1:8">
-      <c r="B128" s="139" t="s">
+      <c r="B128" s="124" t="s">
         <v>126</v>
       </c>
-      <c r="C128" s="137" t="s">
+      <c r="C128" s="127" t="s">
         <v>123</v>
       </c>
       <c r="D128" s="4" t="s">
@@ -34703,16 +34703,16 @@
       <c r="F128" s="4">
         <v>10.5</v>
       </c>
-      <c r="G128" s="137" t="s">
+      <c r="G128" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H128" s="137" t="s">
+      <c r="H128" s="127" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="129" spans="2:8">
-      <c r="B129" s="140"/>
-      <c r="C129" s="142"/>
+      <c r="B129" s="125"/>
+      <c r="C129" s="128"/>
       <c r="D129" s="4" t="s">
         <v>127</v>
       </c>
@@ -34720,21 +34720,21 @@
         <v>101</v>
       </c>
       <c r="F129" s="4"/>
-      <c r="G129" s="142"/>
-      <c r="H129" s="142"/>
+      <c r="G129" s="128"/>
+      <c r="H129" s="128"/>
     </row>
     <row r="130" spans="2:8">
-      <c r="B130" s="140"/>
-      <c r="C130" s="142"/>
+      <c r="B130" s="125"/>
+      <c r="C130" s="128"/>
       <c r="D130" s="11"/>
       <c r="E130" s="4"/>
       <c r="F130" s="4"/>
-      <c r="G130" s="142"/>
-      <c r="H130" s="142"/>
+      <c r="G130" s="128"/>
+      <c r="H130" s="128"/>
     </row>
     <row r="131" spans="2:8" ht="16" thickBot="1">
-      <c r="B131" s="141"/>
-      <c r="C131" s="138"/>
+      <c r="B131" s="126"/>
+      <c r="C131" s="129"/>
       <c r="D131" s="12"/>
       <c r="E131" s="2">
         <v>7.2</v>
@@ -34742,8 +34742,8 @@
       <c r="F131" s="2">
         <v>16.2</v>
       </c>
-      <c r="G131" s="138"/>
-      <c r="H131" s="138"/>
+      <c r="G131" s="129"/>
+      <c r="H131" s="129"/>
     </row>
     <row r="132" spans="2:8" ht="16" thickBot="1">
       <c r="B132" s="1" t="s">
@@ -34769,10 +34769,10 @@
       </c>
     </row>
     <row r="133" spans="2:8" ht="44">
-      <c r="B133" s="139" t="s">
+      <c r="B133" s="124" t="s">
         <v>130</v>
       </c>
-      <c r="C133" s="137" t="s">
+      <c r="C133" s="127" t="s">
         <v>131</v>
       </c>
       <c r="D133" s="5" t="s">
@@ -34781,10 +34781,10 @@
       <c r="E133" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F133" s="137" t="s">
+      <c r="F133" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="G133" s="137" t="s">
+      <c r="G133" s="127" t="s">
         <v>24</v>
       </c>
       <c r="H133" s="4" t="s">
@@ -34792,128 +34792,128 @@
       </c>
     </row>
     <row r="134" spans="2:8">
-      <c r="B134" s="140"/>
-      <c r="C134" s="142"/>
+      <c r="B134" s="125"/>
+      <c r="C134" s="128"/>
       <c r="D134" s="5" t="s">
         <v>133</v>
       </c>
       <c r="E134" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F134" s="142"/>
-      <c r="G134" s="142"/>
+      <c r="F134" s="128"/>
+      <c r="G134" s="128"/>
       <c r="H134" s="4" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="135" spans="2:8">
-      <c r="B135" s="140"/>
-      <c r="C135" s="142"/>
+      <c r="B135" s="125"/>
+      <c r="C135" s="128"/>
       <c r="D135" s="4"/>
       <c r="E135" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F135" s="142"/>
-      <c r="G135" s="142"/>
+      <c r="F135" s="128"/>
+      <c r="G135" s="128"/>
       <c r="H135" s="4" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="136" spans="2:8" ht="179" customHeight="1">
-      <c r="B136" s="140"/>
-      <c r="C136" s="142"/>
+      <c r="B136" s="125"/>
+      <c r="C136" s="128"/>
       <c r="D136" s="5" t="s">
         <v>134</v>
       </c>
       <c r="E136" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F136" s="142"/>
-      <c r="G136" s="142"/>
+      <c r="F136" s="128"/>
+      <c r="G136" s="128"/>
       <c r="H136" s="4" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="137" spans="2:8">
-      <c r="B137" s="140"/>
-      <c r="C137" s="142"/>
+      <c r="B137" s="125"/>
+      <c r="C137" s="128"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F137" s="142"/>
-      <c r="G137" s="142"/>
+      <c r="F137" s="128"/>
+      <c r="G137" s="128"/>
       <c r="H137" s="11"/>
     </row>
     <row r="138" spans="2:8">
-      <c r="B138" s="140"/>
-      <c r="C138" s="142"/>
+      <c r="B138" s="125"/>
+      <c r="C138" s="128"/>
       <c r="D138" s="5" t="s">
         <v>135</v>
       </c>
       <c r="E138" s="4"/>
-      <c r="F138" s="142"/>
-      <c r="G138" s="142"/>
+      <c r="F138" s="128"/>
+      <c r="G138" s="128"/>
       <c r="H138" s="11"/>
     </row>
     <row r="139" spans="2:8" ht="33">
-      <c r="B139" s="140"/>
-      <c r="C139" s="142"/>
+      <c r="B139" s="125"/>
+      <c r="C139" s="128"/>
       <c r="D139" s="11"/>
       <c r="E139" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F139" s="142"/>
-      <c r="G139" s="142"/>
+      <c r="F139" s="128"/>
+      <c r="G139" s="128"/>
       <c r="H139" s="11"/>
     </row>
     <row r="140" spans="2:8">
-      <c r="B140" s="140"/>
-      <c r="C140" s="142"/>
+      <c r="B140" s="125"/>
+      <c r="C140" s="128"/>
       <c r="D140" s="11"/>
       <c r="E140" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F140" s="142"/>
-      <c r="G140" s="142"/>
+      <c r="F140" s="128"/>
+      <c r="G140" s="128"/>
       <c r="H140" s="11"/>
     </row>
     <row r="141" spans="2:8">
-      <c r="B141" s="140"/>
-      <c r="C141" s="142"/>
+      <c r="B141" s="125"/>
+      <c r="C141" s="128"/>
       <c r="D141" s="11"/>
       <c r="E141" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F141" s="142"/>
-      <c r="G141" s="142"/>
+      <c r="F141" s="128"/>
+      <c r="G141" s="128"/>
       <c r="H141" s="11"/>
     </row>
     <row r="142" spans="2:8">
-      <c r="B142" s="140"/>
-      <c r="C142" s="142"/>
+      <c r="B142" s="125"/>
+      <c r="C142" s="128"/>
       <c r="D142" s="11"/>
       <c r="E142" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F142" s="142"/>
-      <c r="G142" s="142"/>
+      <c r="F142" s="128"/>
+      <c r="G142" s="128"/>
       <c r="H142" s="11"/>
     </row>
     <row r="143" spans="2:8" ht="16" thickBot="1">
-      <c r="B143" s="141"/>
-      <c r="C143" s="138"/>
+      <c r="B143" s="126"/>
+      <c r="C143" s="129"/>
       <c r="D143" s="12"/>
       <c r="E143" s="2"/>
-      <c r="F143" s="138"/>
-      <c r="G143" s="138"/>
+      <c r="F143" s="129"/>
+      <c r="G143" s="129"/>
       <c r="H143" s="12"/>
     </row>
     <row r="144" spans="2:8">
-      <c r="B144" s="139" t="s">
+      <c r="B144" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="C144" s="137" t="s">
+      <c r="C144" s="127" t="s">
         <v>131</v>
       </c>
       <c r="D144" s="4" t="s">
@@ -34933,8 +34933,8 @@
       </c>
     </row>
     <row r="145" spans="1:8" ht="23" thickBot="1">
-      <c r="B145" s="141"/>
-      <c r="C145" s="138"/>
+      <c r="B145" s="126"/>
+      <c r="C145" s="129"/>
       <c r="D145" s="13" t="s">
         <v>150</v>
       </c>
@@ -34955,15 +34955,15 @@
       <c r="B146" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C146" s="137" t="s">
+      <c r="C146" s="127" t="s">
         <v>131</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E146" s="137"/>
-      <c r="F146" s="137"/>
-      <c r="G146" s="137"/>
+      <c r="E146" s="127"/>
+      <c r="F146" s="127"/>
+      <c r="G146" s="127"/>
       <c r="H146" s="4" t="s">
         <v>156</v>
       </c>
@@ -34973,35 +34973,35 @@
       <c r="B147" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C147" s="142"/>
+      <c r="C147" s="128"/>
       <c r="D147" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E147" s="142"/>
-      <c r="F147" s="142"/>
-      <c r="G147" s="142"/>
+      <c r="E147" s="128"/>
+      <c r="F147" s="128"/>
+      <c r="G147" s="128"/>
       <c r="H147" s="4" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="88">
       <c r="B148" s="114"/>
-      <c r="C148" s="142"/>
+      <c r="C148" s="128"/>
       <c r="D148" s="4"/>
-      <c r="E148" s="142"/>
-      <c r="F148" s="142"/>
-      <c r="G148" s="142"/>
+      <c r="E148" s="128"/>
+      <c r="F148" s="128"/>
+      <c r="G148" s="128"/>
       <c r="H148" s="4" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="16" thickBot="1">
       <c r="B149" s="115"/>
-      <c r="C149" s="138"/>
+      <c r="C149" s="129"/>
       <c r="D149" s="12"/>
-      <c r="E149" s="138"/>
-      <c r="F149" s="138"/>
-      <c r="G149" s="138"/>
+      <c r="E149" s="129"/>
+      <c r="F149" s="129"/>
+      <c r="G149" s="129"/>
       <c r="H149" s="2" t="s">
         <v>159</v>
       </c>
@@ -35028,137 +35028,137 @@
       <c r="H150" s="2"/>
     </row>
     <row r="151" spans="1:8" ht="28" customHeight="1">
-      <c r="B151" s="139" t="s">
+      <c r="B151" s="124" t="s">
         <v>164</v>
       </c>
-      <c r="C151" s="137" t="s">
+      <c r="C151" s="127" t="s">
         <v>131</v>
       </c>
-      <c r="D151" s="137" t="s">
+      <c r="D151" s="127" t="s">
         <v>165</v>
       </c>
       <c r="E151" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F151" s="137" t="s">
+      <c r="F151" s="127" t="s">
         <v>168</v>
       </c>
-      <c r="G151" s="137" t="s">
+      <c r="G151" s="127" t="s">
         <v>169</v>
       </c>
-      <c r="H151" s="137"/>
+      <c r="H151" s="127"/>
     </row>
     <row r="152" spans="1:8" ht="16" thickBot="1">
-      <c r="B152" s="141"/>
-      <c r="C152" s="138"/>
-      <c r="D152" s="138"/>
+      <c r="B152" s="126"/>
+      <c r="C152" s="129"/>
+      <c r="D152" s="129"/>
       <c r="E152" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F152" s="138"/>
-      <c r="G152" s="138"/>
-      <c r="H152" s="138"/>
+      <c r="F152" s="129"/>
+      <c r="G152" s="129"/>
+      <c r="H152" s="129"/>
     </row>
     <row r="153" spans="1:8">
-      <c r="B153" s="120"/>
-      <c r="C153" s="121"/>
-      <c r="D153" s="121"/>
-      <c r="E153" s="121"/>
-      <c r="F153" s="121"/>
-      <c r="G153" s="121"/>
-      <c r="H153" s="122"/>
+      <c r="B153" s="143"/>
+      <c r="C153" s="144"/>
+      <c r="D153" s="144"/>
+      <c r="E153" s="144"/>
+      <c r="F153" s="144"/>
+      <c r="G153" s="144"/>
+      <c r="H153" s="145"/>
     </row>
     <row r="154" spans="1:8">
-      <c r="B154" s="123" t="s">
+      <c r="B154" s="146" t="s">
         <v>170</v>
       </c>
-      <c r="C154" s="124"/>
-      <c r="D154" s="124"/>
-      <c r="E154" s="124"/>
-      <c r="F154" s="124"/>
-      <c r="G154" s="124"/>
-      <c r="H154" s="125"/>
+      <c r="C154" s="147"/>
+      <c r="D154" s="147"/>
+      <c r="E154" s="147"/>
+      <c r="F154" s="147"/>
+      <c r="G154" s="147"/>
+      <c r="H154" s="148"/>
     </row>
     <row r="155" spans="1:8" ht="16" thickBot="1">
-      <c r="B155" s="126"/>
-      <c r="C155" s="127"/>
-      <c r="D155" s="127"/>
-      <c r="E155" s="127"/>
-      <c r="F155" s="127"/>
-      <c r="G155" s="127"/>
-      <c r="H155" s="128"/>
+      <c r="B155" s="149"/>
+      <c r="C155" s="150"/>
+      <c r="D155" s="150"/>
+      <c r="E155" s="150"/>
+      <c r="F155" s="150"/>
+      <c r="G155" s="150"/>
+      <c r="H155" s="151"/>
     </row>
     <row r="156" spans="1:8" ht="44" customHeight="1">
-      <c r="B156" s="139" t="s">
+      <c r="B156" s="124" t="s">
         <v>171</v>
       </c>
-      <c r="C156" s="137" t="s">
+      <c r="C156" s="127" t="s">
         <v>172</v>
       </c>
-      <c r="D156" s="150" t="s">
+      <c r="D156" s="158" t="s">
         <v>56</v>
       </c>
       <c r="E156" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="F156" s="137" t="s">
+      <c r="F156" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="G156" s="137" t="s">
+      <c r="G156" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H156" s="137" t="s">
+      <c r="H156" s="127" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="157" spans="1:8">
-      <c r="B157" s="140"/>
-      <c r="C157" s="142"/>
-      <c r="D157" s="151"/>
+      <c r="B157" s="125"/>
+      <c r="C157" s="128"/>
+      <c r="D157" s="163"/>
       <c r="E157" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="F157" s="142"/>
-      <c r="G157" s="142"/>
-      <c r="H157" s="142"/>
+      <c r="F157" s="128"/>
+      <c r="G157" s="128"/>
+      <c r="H157" s="128"/>
     </row>
     <row r="158" spans="1:8">
-      <c r="B158" s="140"/>
-      <c r="C158" s="142"/>
-      <c r="D158" s="151"/>
+      <c r="B158" s="125"/>
+      <c r="C158" s="128"/>
+      <c r="D158" s="163"/>
       <c r="E158" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="F158" s="142"/>
-      <c r="G158" s="142"/>
-      <c r="H158" s="142"/>
+      <c r="F158" s="128"/>
+      <c r="G158" s="128"/>
+      <c r="H158" s="128"/>
     </row>
     <row r="159" spans="1:8" ht="16" thickBot="1">
-      <c r="B159" s="141"/>
-      <c r="C159" s="138"/>
-      <c r="D159" s="152"/>
+      <c r="B159" s="126"/>
+      <c r="C159" s="129"/>
+      <c r="D159" s="159"/>
       <c r="E159" s="2"/>
-      <c r="F159" s="138"/>
-      <c r="G159" s="138"/>
-      <c r="H159" s="138"/>
+      <c r="F159" s="129"/>
+      <c r="G159" s="129"/>
+      <c r="H159" s="129"/>
     </row>
     <row r="160" spans="1:8" ht="44">
-      <c r="B160" s="139" t="s">
+      <c r="B160" s="124" t="s">
         <v>177</v>
       </c>
-      <c r="C160" s="137" t="s">
+      <c r="C160" s="127" t="s">
         <v>178</v>
       </c>
-      <c r="D160" s="137" t="s">
+      <c r="D160" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="E160" s="137" t="s">
+      <c r="E160" s="127" t="s">
         <v>24</v>
       </c>
       <c r="F160" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="G160" s="137" t="s">
+      <c r="G160" s="127" t="s">
         <v>24</v>
       </c>
       <c r="H160" s="4" t="s">
@@ -35166,25 +35166,25 @@
       </c>
     </row>
     <row r="161" spans="1:8">
-      <c r="B161" s="140"/>
-      <c r="C161" s="142"/>
-      <c r="D161" s="142"/>
-      <c r="E161" s="142"/>
+      <c r="B161" s="125"/>
+      <c r="C161" s="128"/>
+      <c r="D161" s="128"/>
+      <c r="E161" s="128"/>
       <c r="F161" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="G161" s="142"/>
+      <c r="G161" s="128"/>
       <c r="H161" s="4" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="162" spans="1:8" ht="56" thickBot="1">
-      <c r="B162" s="141"/>
-      <c r="C162" s="138"/>
-      <c r="D162" s="138"/>
-      <c r="E162" s="138"/>
+      <c r="B162" s="126"/>
+      <c r="C162" s="129"/>
+      <c r="D162" s="129"/>
+      <c r="E162" s="129"/>
       <c r="F162" s="12"/>
-      <c r="G162" s="138"/>
+      <c r="G162" s="129"/>
       <c r="H162" s="2" t="s">
         <v>183</v>
       </c>
@@ -35210,22 +35210,22 @@
       <c r="B164" s="111" t="s">
         <v>185</v>
       </c>
-      <c r="C164" s="135" t="s">
+      <c r="C164" s="130" t="s">
         <v>2447</v>
       </c>
-      <c r="D164" s="133" t="s">
+      <c r="D164" s="132" t="s">
         <v>187</v>
       </c>
-      <c r="E164" s="148">
+      <c r="E164" s="134">
         <v>0.33</v>
       </c>
-      <c r="F164" s="148">
+      <c r="F164" s="134">
         <v>0.33</v>
       </c>
-      <c r="G164" s="148">
+      <c r="G164" s="134">
         <v>0.33</v>
       </c>
-      <c r="H164" s="148">
+      <c r="H164" s="134">
         <v>0.33</v>
       </c>
     </row>
@@ -35233,51 +35233,51 @@
       <c r="B165" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="C165" s="136"/>
-      <c r="D165" s="134"/>
-      <c r="E165" s="149"/>
-      <c r="F165" s="149"/>
-      <c r="G165" s="149"/>
-      <c r="H165" s="149"/>
+      <c r="C165" s="131"/>
+      <c r="D165" s="133"/>
+      <c r="E165" s="135"/>
+      <c r="F165" s="135"/>
+      <c r="G165" s="135"/>
+      <c r="H165" s="135"/>
     </row>
     <row r="166" spans="1:8">
       <c r="A166" s="20"/>
-      <c r="B166" s="120"/>
-      <c r="C166" s="121"/>
-      <c r="D166" s="121"/>
-      <c r="E166" s="121"/>
-      <c r="F166" s="121"/>
-      <c r="G166" s="121"/>
-      <c r="H166" s="122"/>
+      <c r="B166" s="143"/>
+      <c r="C166" s="144"/>
+      <c r="D166" s="144"/>
+      <c r="E166" s="144"/>
+      <c r="F166" s="144"/>
+      <c r="G166" s="144"/>
+      <c r="H166" s="145"/>
     </row>
     <row r="167" spans="1:8">
       <c r="A167" s="20"/>
-      <c r="B167" s="123" t="s">
+      <c r="B167" s="146" t="s">
         <v>188</v>
       </c>
-      <c r="C167" s="124"/>
-      <c r="D167" s="124"/>
-      <c r="E167" s="124"/>
-      <c r="F167" s="124"/>
-      <c r="G167" s="124"/>
-      <c r="H167" s="125"/>
+      <c r="C167" s="147"/>
+      <c r="D167" s="147"/>
+      <c r="E167" s="147"/>
+      <c r="F167" s="147"/>
+      <c r="G167" s="147"/>
+      <c r="H167" s="148"/>
     </row>
     <row r="168" spans="1:8" ht="16" thickBot="1">
       <c r="A168" s="20"/>
-      <c r="B168" s="126"/>
-      <c r="C168" s="127"/>
-      <c r="D168" s="127"/>
-      <c r="E168" s="127"/>
-      <c r="F168" s="127"/>
-      <c r="G168" s="127"/>
-      <c r="H168" s="128"/>
+      <c r="B168" s="149"/>
+      <c r="C168" s="150"/>
+      <c r="D168" s="150"/>
+      <c r="E168" s="150"/>
+      <c r="F168" s="150"/>
+      <c r="G168" s="150"/>
+      <c r="H168" s="151"/>
     </row>
     <row r="169" spans="1:8">
       <c r="A169" s="20"/>
-      <c r="B169" s="129" t="s">
+      <c r="B169" s="136" t="s">
         <v>189</v>
       </c>
-      <c r="C169" s="135" t="s">
+      <c r="C169" s="130" t="s">
         <v>190</v>
       </c>
       <c r="D169" s="6" t="s">
@@ -35286,50 +35286,50 @@
       <c r="E169" s="16">
         <v>0.44</v>
       </c>
-      <c r="F169" s="135" t="s">
+      <c r="F169" s="130" t="s">
         <v>194</v>
       </c>
-      <c r="G169" s="135" t="s">
+      <c r="G169" s="130" t="s">
         <v>194</v>
       </c>
-      <c r="H169" s="135" t="s">
+      <c r="H169" s="130" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="170" spans="1:8">
       <c r="A170" s="20"/>
-      <c r="B170" s="146"/>
-      <c r="C170" s="147"/>
+      <c r="B170" s="137"/>
+      <c r="C170" s="139"/>
       <c r="D170" s="9" t="s">
         <v>192</v>
       </c>
       <c r="E170" s="6"/>
-      <c r="F170" s="147"/>
-      <c r="G170" s="147"/>
-      <c r="H170" s="147"/>
+      <c r="F170" s="139"/>
+      <c r="G170" s="139"/>
+      <c r="H170" s="139"/>
     </row>
     <row r="171" spans="1:8">
       <c r="A171" s="20"/>
-      <c r="B171" s="146"/>
-      <c r="C171" s="147"/>
+      <c r="B171" s="137"/>
+      <c r="C171" s="139"/>
       <c r="D171" s="6"/>
       <c r="E171" s="16">
         <v>0.41</v>
       </c>
-      <c r="F171" s="147"/>
-      <c r="G171" s="147"/>
-      <c r="H171" s="147"/>
+      <c r="F171" s="139"/>
+      <c r="G171" s="139"/>
+      <c r="H171" s="139"/>
     </row>
     <row r="172" spans="1:8" ht="16" thickBot="1">
-      <c r="B172" s="130"/>
-      <c r="C172" s="136"/>
+      <c r="B172" s="138"/>
+      <c r="C172" s="131"/>
       <c r="D172" s="14" t="s">
         <v>193</v>
       </c>
       <c r="E172" s="10"/>
-      <c r="F172" s="136"/>
-      <c r="G172" s="136"/>
-      <c r="H172" s="136"/>
+      <c r="F172" s="131"/>
+      <c r="G172" s="131"/>
+      <c r="H172" s="131"/>
     </row>
     <row r="173" spans="1:8" ht="34" thickBot="1">
       <c r="B173" s="112" t="s">
@@ -35355,39 +35355,39 @@
       </c>
     </row>
     <row r="174" spans="1:8" ht="164" customHeight="1">
-      <c r="B174" s="129" t="s">
+      <c r="B174" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="C174" s="135" t="s">
+      <c r="C174" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="D174" s="133" t="s">
+      <c r="D174" s="132" t="s">
         <v>200</v>
       </c>
-      <c r="E174" s="135" t="s">
+      <c r="E174" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="F174" s="135" t="s">
+      <c r="F174" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="G174" s="135" t="s">
+      <c r="G174" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="H174" s="135" t="s">
+      <c r="H174" s="130" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="175" spans="1:8" ht="16" thickBot="1">
-      <c r="B175" s="130"/>
-      <c r="C175" s="136"/>
-      <c r="D175" s="134"/>
-      <c r="E175" s="136"/>
-      <c r="F175" s="136"/>
-      <c r="G175" s="136"/>
-      <c r="H175" s="136"/>
+      <c r="B175" s="138"/>
+      <c r="C175" s="131"/>
+      <c r="D175" s="133"/>
+      <c r="E175" s="131"/>
+      <c r="F175" s="131"/>
+      <c r="G175" s="131"/>
+      <c r="H175" s="131"/>
     </row>
     <row r="176" spans="1:8" ht="33">
-      <c r="B176" s="129" t="s">
+      <c r="B176" s="136" t="s">
         <v>202</v>
       </c>
       <c r="C176" s="6" t="s">
@@ -35399,10 +35399,10 @@
       <c r="E176" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F176" s="135" t="s">
+      <c r="F176" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="G176" s="135" t="s">
+      <c r="G176" s="130" t="s">
         <v>176</v>
       </c>
       <c r="H176" s="6" t="s">
@@ -35410,7 +35410,7 @@
       </c>
     </row>
     <row r="177" spans="2:8" ht="99">
-      <c r="B177" s="146"/>
+      <c r="B177" s="137"/>
       <c r="C177" s="6" t="s">
         <v>203</v>
       </c>
@@ -35418,49 +35418,49 @@
       <c r="E177" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="F177" s="147"/>
-      <c r="G177" s="147"/>
+      <c r="F177" s="139"/>
+      <c r="G177" s="139"/>
       <c r="H177" s="6" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="178" spans="2:8">
-      <c r="B178" s="146"/>
+      <c r="B178" s="137"/>
       <c r="C178" s="6"/>
       <c r="D178" s="9" t="s">
         <v>4</v>
       </c>
       <c r="E178" s="7"/>
-      <c r="F178" s="147"/>
-      <c r="G178" s="147"/>
+      <c r="F178" s="139"/>
+      <c r="G178" s="139"/>
       <c r="H178" s="6" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="179" spans="2:8">
-      <c r="B179" s="146"/>
+      <c r="B179" s="137"/>
       <c r="C179" s="7"/>
       <c r="D179" s="9" t="s">
         <v>205</v>
       </c>
       <c r="E179" s="7"/>
-      <c r="F179" s="147"/>
-      <c r="G179" s="147"/>
+      <c r="F179" s="139"/>
+      <c r="G179" s="139"/>
       <c r="H179" s="6" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="180" spans="2:8" ht="16" thickBot="1">
-      <c r="B180" s="130"/>
+      <c r="B180" s="138"/>
       <c r="C180" s="8"/>
       <c r="D180" s="10"/>
       <c r="E180" s="8"/>
-      <c r="F180" s="136"/>
-      <c r="G180" s="136"/>
+      <c r="F180" s="131"/>
+      <c r="G180" s="131"/>
       <c r="H180" s="10"/>
     </row>
     <row r="181" spans="2:8" ht="30">
-      <c r="B181" s="129" t="s">
+      <c r="B181" s="136" t="s">
         <v>210</v>
       </c>
       <c r="C181" s="6" t="s">
@@ -35469,13 +35469,13 @@
       <c r="D181" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="E181" s="135" t="s">
+      <c r="E181" s="130" t="s">
         <v>214</v>
       </c>
-      <c r="F181" s="135" t="s">
+      <c r="F181" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="G181" s="135" t="s">
+      <c r="G181" s="130" t="s">
         <v>24</v>
       </c>
       <c r="H181" s="6" t="s">
@@ -35483,40 +35483,40 @@
       </c>
     </row>
     <row r="182" spans="2:8" ht="55">
-      <c r="B182" s="146"/>
+      <c r="B182" s="137"/>
       <c r="C182" s="6" t="s">
         <v>212</v>
       </c>
       <c r="D182" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E182" s="147"/>
-      <c r="F182" s="147"/>
-      <c r="G182" s="147"/>
+      <c r="E182" s="139"/>
+      <c r="F182" s="139"/>
+      <c r="G182" s="139"/>
       <c r="H182" s="6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="183" spans="2:8">
-      <c r="B183" s="146"/>
+      <c r="B183" s="137"/>
       <c r="C183" s="6"/>
       <c r="D183" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="E183" s="147"/>
-      <c r="F183" s="147"/>
-      <c r="G183" s="147"/>
+      <c r="E183" s="139"/>
+      <c r="F183" s="139"/>
+      <c r="G183" s="139"/>
       <c r="H183" s="6" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="184" spans="2:8" ht="16" thickBot="1">
-      <c r="B184" s="130"/>
+      <c r="B184" s="138"/>
       <c r="C184" s="8"/>
       <c r="D184" s="10"/>
-      <c r="E184" s="136"/>
-      <c r="F184" s="136"/>
-      <c r="G184" s="136"/>
+      <c r="E184" s="131"/>
+      <c r="F184" s="131"/>
+      <c r="G184" s="131"/>
       <c r="H184" s="8"/>
     </row>
     <row r="185" spans="2:8" ht="16" thickBot="1">
@@ -35539,107 +35539,107 @@
       </c>
     </row>
     <row r="186" spans="2:8">
-      <c r="B186" s="120"/>
-      <c r="C186" s="121"/>
-      <c r="D186" s="121"/>
-      <c r="E186" s="121"/>
-      <c r="F186" s="121"/>
-      <c r="G186" s="121"/>
-      <c r="H186" s="122"/>
+      <c r="B186" s="143"/>
+      <c r="C186" s="144"/>
+      <c r="D186" s="144"/>
+      <c r="E186" s="144"/>
+      <c r="F186" s="144"/>
+      <c r="G186" s="144"/>
+      <c r="H186" s="145"/>
     </row>
     <row r="187" spans="2:8">
-      <c r="B187" s="123" t="s">
+      <c r="B187" s="146" t="s">
         <v>219</v>
       </c>
-      <c r="C187" s="124"/>
-      <c r="D187" s="124"/>
-      <c r="E187" s="124"/>
-      <c r="F187" s="124"/>
-      <c r="G187" s="124"/>
-      <c r="H187" s="125"/>
+      <c r="C187" s="147"/>
+      <c r="D187" s="147"/>
+      <c r="E187" s="147"/>
+      <c r="F187" s="147"/>
+      <c r="G187" s="147"/>
+      <c r="H187" s="148"/>
     </row>
     <row r="188" spans="2:8" ht="16" thickBot="1">
-      <c r="B188" s="126"/>
-      <c r="C188" s="127"/>
-      <c r="D188" s="127"/>
-      <c r="E188" s="127"/>
-      <c r="F188" s="127"/>
-      <c r="G188" s="127"/>
-      <c r="H188" s="128"/>
+      <c r="B188" s="149"/>
+      <c r="C188" s="150"/>
+      <c r="D188" s="150"/>
+      <c r="E188" s="150"/>
+      <c r="F188" s="150"/>
+      <c r="G188" s="150"/>
+      <c r="H188" s="151"/>
     </row>
     <row r="189" spans="2:8" ht="30">
-      <c r="B189" s="139" t="s">
+      <c r="B189" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="C189" s="137"/>
+      <c r="C189" s="127"/>
       <c r="D189" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E189" s="137" t="s">
+      <c r="E189" s="127" t="s">
         <v>223</v>
       </c>
       <c r="F189" s="17">
         <v>1805853</v>
       </c>
-      <c r="G189" s="137" t="s">
+      <c r="G189" s="127" t="s">
         <v>225</v>
       </c>
-      <c r="H189" s="137" t="s">
+      <c r="H189" s="127" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="190" spans="2:8" ht="30">
-      <c r="B190" s="140"/>
-      <c r="C190" s="142"/>
+      <c r="B190" s="125"/>
+      <c r="C190" s="128"/>
       <c r="D190" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="E190" s="142"/>
+      <c r="E190" s="128"/>
       <c r="F190" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="G190" s="142"/>
-      <c r="H190" s="142"/>
+      <c r="G190" s="128"/>
+      <c r="H190" s="128"/>
     </row>
     <row r="191" spans="2:8" ht="30">
-      <c r="B191" s="140"/>
-      <c r="C191" s="142"/>
+      <c r="B191" s="125"/>
+      <c r="C191" s="128"/>
       <c r="D191" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="E191" s="142"/>
+      <c r="E191" s="128"/>
       <c r="F191" s="4"/>
-      <c r="G191" s="142"/>
-      <c r="H191" s="142"/>
+      <c r="G191" s="128"/>
+      <c r="H191" s="128"/>
     </row>
     <row r="192" spans="2:8">
-      <c r="B192" s="140"/>
-      <c r="C192" s="142"/>
+      <c r="B192" s="125"/>
+      <c r="C192" s="128"/>
       <c r="D192" s="4"/>
-      <c r="E192" s="142"/>
+      <c r="E192" s="128"/>
       <c r="F192" s="4"/>
-      <c r="G192" s="142"/>
-      <c r="H192" s="142"/>
+      <c r="G192" s="128"/>
+      <c r="H192" s="128"/>
     </row>
     <row r="193" spans="2:8" ht="30">
-      <c r="B193" s="140"/>
-      <c r="C193" s="142"/>
+      <c r="B193" s="125"/>
+      <c r="C193" s="128"/>
       <c r="D193" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="E193" s="142"/>
+      <c r="E193" s="128"/>
       <c r="F193" s="4"/>
-      <c r="G193" s="142"/>
-      <c r="H193" s="142"/>
+      <c r="G193" s="128"/>
+      <c r="H193" s="128"/>
     </row>
     <row r="194" spans="2:8" ht="16" thickBot="1">
-      <c r="B194" s="141"/>
-      <c r="C194" s="138"/>
+      <c r="B194" s="126"/>
+      <c r="C194" s="129"/>
       <c r="D194" s="12"/>
-      <c r="E194" s="138"/>
+      <c r="E194" s="129"/>
       <c r="F194" s="2"/>
-      <c r="G194" s="138"/>
-      <c r="H194" s="138"/>
+      <c r="G194" s="129"/>
+      <c r="H194" s="129"/>
     </row>
     <row r="195" spans="2:8" ht="31" thickBot="1">
       <c r="B195" s="1" t="s">
@@ -35663,141 +35663,141 @@
       </c>
     </row>
     <row r="196" spans="2:8">
-      <c r="B196" s="139" t="s">
+      <c r="B196" s="124" t="s">
         <v>230</v>
       </c>
-      <c r="C196" s="137"/>
+      <c r="C196" s="127"/>
       <c r="D196" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="E196" s="137">
+      <c r="E196" s="127">
         <v>0.86</v>
       </c>
-      <c r="F196" s="137">
+      <c r="F196" s="127">
         <v>0.79</v>
       </c>
-      <c r="G196" s="137">
+      <c r="G196" s="127">
         <v>0.71</v>
       </c>
-      <c r="H196" s="137">
+      <c r="H196" s="127">
         <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="197" spans="2:8" ht="16" thickBot="1">
-      <c r="B197" s="141"/>
-      <c r="C197" s="138"/>
+      <c r="B197" s="126"/>
+      <c r="C197" s="129"/>
       <c r="D197" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="E197" s="138"/>
-      <c r="F197" s="138"/>
-      <c r="G197" s="138"/>
-      <c r="H197" s="138"/>
+      <c r="E197" s="129"/>
+      <c r="F197" s="129"/>
+      <c r="G197" s="129"/>
+      <c r="H197" s="129"/>
     </row>
     <row r="198" spans="2:8">
-      <c r="B198" s="120"/>
-      <c r="C198" s="121"/>
-      <c r="D198" s="121"/>
-      <c r="E198" s="121"/>
-      <c r="F198" s="121"/>
-      <c r="G198" s="121"/>
-      <c r="H198" s="122"/>
+      <c r="B198" s="143"/>
+      <c r="C198" s="144"/>
+      <c r="D198" s="144"/>
+      <c r="E198" s="144"/>
+      <c r="F198" s="144"/>
+      <c r="G198" s="144"/>
+      <c r="H198" s="145"/>
     </row>
     <row r="199" spans="2:8">
-      <c r="B199" s="123" t="s">
+      <c r="B199" s="146" t="s">
         <v>233</v>
       </c>
-      <c r="C199" s="124"/>
-      <c r="D199" s="124"/>
-      <c r="E199" s="124"/>
-      <c r="F199" s="124"/>
-      <c r="G199" s="124"/>
-      <c r="H199" s="125"/>
+      <c r="C199" s="147"/>
+      <c r="D199" s="147"/>
+      <c r="E199" s="147"/>
+      <c r="F199" s="147"/>
+      <c r="G199" s="147"/>
+      <c r="H199" s="148"/>
     </row>
     <row r="200" spans="2:8" ht="16" thickBot="1">
-      <c r="B200" s="126"/>
-      <c r="C200" s="127"/>
-      <c r="D200" s="127"/>
-      <c r="E200" s="127"/>
-      <c r="F200" s="127"/>
-      <c r="G200" s="127"/>
-      <c r="H200" s="128"/>
+      <c r="B200" s="149"/>
+      <c r="C200" s="150"/>
+      <c r="D200" s="150"/>
+      <c r="E200" s="150"/>
+      <c r="F200" s="150"/>
+      <c r="G200" s="150"/>
+      <c r="H200" s="151"/>
     </row>
     <row r="201" spans="2:8" ht="30">
-      <c r="B201" s="139" t="s">
+      <c r="B201" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C201" s="137" t="s">
+      <c r="C201" s="127" t="s">
         <v>235</v>
       </c>
       <c r="D201" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="E201" s="137" t="s">
+      <c r="E201" s="127" t="s">
         <v>24</v>
       </c>
       <c r="F201" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="G201" s="137" t="s">
+      <c r="G201" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H201" s="143" t="s">
+      <c r="H201" s="164" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="202" spans="2:8" ht="22">
-      <c r="B202" s="140"/>
-      <c r="C202" s="142"/>
+      <c r="B202" s="125"/>
+      <c r="C202" s="128"/>
       <c r="D202" s="4"/>
-      <c r="E202" s="142"/>
+      <c r="E202" s="128"/>
       <c r="F202" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="G202" s="142"/>
-      <c r="H202" s="144"/>
+      <c r="G202" s="128"/>
+      <c r="H202" s="165"/>
     </row>
     <row r="203" spans="2:8" ht="23" thickBot="1">
-      <c r="B203" s="141"/>
-      <c r="C203" s="138"/>
+      <c r="B203" s="126"/>
+      <c r="C203" s="129"/>
       <c r="D203" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="E203" s="138"/>
+      <c r="E203" s="129"/>
       <c r="F203" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="G203" s="138"/>
-      <c r="H203" s="145"/>
+      <c r="G203" s="129"/>
+      <c r="H203" s="166"/>
     </row>
     <row r="204" spans="2:8">
-      <c r="B204" s="120"/>
-      <c r="C204" s="121"/>
-      <c r="D204" s="121"/>
-      <c r="E204" s="121"/>
-      <c r="F204" s="121"/>
-      <c r="G204" s="121"/>
-      <c r="H204" s="122"/>
+      <c r="B204" s="143"/>
+      <c r="C204" s="144"/>
+      <c r="D204" s="144"/>
+      <c r="E204" s="144"/>
+      <c r="F204" s="144"/>
+      <c r="G204" s="144"/>
+      <c r="H204" s="145"/>
     </row>
     <row r="205" spans="2:8">
-      <c r="B205" s="123" t="s">
+      <c r="B205" s="146" t="s">
         <v>2448</v>
       </c>
-      <c r="C205" s="124"/>
-      <c r="D205" s="124"/>
-      <c r="E205" s="124"/>
-      <c r="F205" s="124"/>
-      <c r="G205" s="124"/>
-      <c r="H205" s="125"/>
+      <c r="C205" s="147"/>
+      <c r="D205" s="147"/>
+      <c r="E205" s="147"/>
+      <c r="F205" s="147"/>
+      <c r="G205" s="147"/>
+      <c r="H205" s="148"/>
     </row>
     <row r="206" spans="2:8" ht="16" thickBot="1">
-      <c r="B206" s="126"/>
-      <c r="C206" s="127"/>
-      <c r="D206" s="127"/>
-      <c r="E206" s="127"/>
-      <c r="F206" s="127"/>
-      <c r="G206" s="127"/>
-      <c r="H206" s="128"/>
+      <c r="B206" s="149"/>
+      <c r="C206" s="150"/>
+      <c r="D206" s="150"/>
+      <c r="E206" s="150"/>
+      <c r="F206" s="150"/>
+      <c r="G206" s="150"/>
+      <c r="H206" s="151"/>
     </row>
     <row r="207" spans="2:8" ht="31" thickBot="1">
       <c r="B207" s="112" t="s">
@@ -35823,36 +35823,36 @@
       </c>
     </row>
     <row r="208" spans="2:8" ht="59" customHeight="1">
-      <c r="B208" s="129" t="s">
+      <c r="B208" s="136" t="s">
         <v>243</v>
       </c>
-      <c r="C208" s="131" t="s">
+      <c r="C208" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="D208" s="133" t="s">
+      <c r="D208" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="E208" s="135" t="s">
+      <c r="E208" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="F208" s="135" t="s">
+      <c r="F208" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="G208" s="135" t="s">
+      <c r="G208" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="H208" s="135">
+      <c r="H208" s="130">
         <v>23</v>
       </c>
     </row>
     <row r="209" spans="2:8" ht="16" thickBot="1">
-      <c r="B209" s="130"/>
-      <c r="C209" s="132"/>
-      <c r="D209" s="134"/>
-      <c r="E209" s="136"/>
-      <c r="F209" s="136"/>
-      <c r="G209" s="136"/>
-      <c r="H209" s="136"/>
+      <c r="B209" s="138"/>
+      <c r="C209" s="168"/>
+      <c r="D209" s="133"/>
+      <c r="E209" s="131"/>
+      <c r="F209" s="131"/>
+      <c r="G209" s="131"/>
+      <c r="H209" s="131"/>
     </row>
     <row r="210" spans="2:8" ht="31" thickBot="1">
       <c r="B210" s="112" t="s">
@@ -35974,6 +35974,208 @@
     </row>
   </sheetData>
   <mergeCells count="226">
+    <mergeCell ref="B204:H204"/>
+    <mergeCell ref="B205:H205"/>
+    <mergeCell ref="B206:H206"/>
+    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="C208:C209"/>
+    <mergeCell ref="D208:D209"/>
+    <mergeCell ref="E208:E209"/>
+    <mergeCell ref="F208:F209"/>
+    <mergeCell ref="G208:G209"/>
+    <mergeCell ref="H208:H209"/>
+    <mergeCell ref="H196:H197"/>
+    <mergeCell ref="B198:H198"/>
+    <mergeCell ref="B199:H199"/>
+    <mergeCell ref="B200:H200"/>
+    <mergeCell ref="B201:B203"/>
+    <mergeCell ref="C201:C203"/>
+    <mergeCell ref="E201:E203"/>
+    <mergeCell ref="G201:G203"/>
+    <mergeCell ref="H201:H203"/>
+    <mergeCell ref="B196:B197"/>
+    <mergeCell ref="C196:C197"/>
+    <mergeCell ref="E196:E197"/>
+    <mergeCell ref="F196:F197"/>
+    <mergeCell ref="G196:G197"/>
+    <mergeCell ref="B187:H187"/>
+    <mergeCell ref="B188:H188"/>
+    <mergeCell ref="B189:B194"/>
+    <mergeCell ref="C189:C194"/>
+    <mergeCell ref="E189:E194"/>
+    <mergeCell ref="G189:G194"/>
+    <mergeCell ref="H189:H194"/>
+    <mergeCell ref="B181:B184"/>
+    <mergeCell ref="E181:E184"/>
+    <mergeCell ref="F181:F184"/>
+    <mergeCell ref="G181:G184"/>
+    <mergeCell ref="B186:H186"/>
+    <mergeCell ref="G174:G175"/>
+    <mergeCell ref="H174:H175"/>
+    <mergeCell ref="B176:B180"/>
+    <mergeCell ref="F176:F180"/>
+    <mergeCell ref="G176:G180"/>
+    <mergeCell ref="B174:B175"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="D174:D175"/>
+    <mergeCell ref="E174:E175"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="B168:H168"/>
+    <mergeCell ref="B169:B172"/>
+    <mergeCell ref="C169:C172"/>
+    <mergeCell ref="F169:F172"/>
+    <mergeCell ref="G169:G172"/>
+    <mergeCell ref="H169:H172"/>
+    <mergeCell ref="F164:F165"/>
+    <mergeCell ref="G164:G165"/>
+    <mergeCell ref="H164:H165"/>
+    <mergeCell ref="B166:H166"/>
+    <mergeCell ref="B167:H167"/>
+    <mergeCell ref="H151:H152"/>
+    <mergeCell ref="B153:H153"/>
+    <mergeCell ref="B154:H154"/>
+    <mergeCell ref="B155:H155"/>
+    <mergeCell ref="B156:B159"/>
+    <mergeCell ref="C156:C159"/>
+    <mergeCell ref="D156:D159"/>
+    <mergeCell ref="F156:F159"/>
+    <mergeCell ref="G156:G159"/>
+    <mergeCell ref="H156:H159"/>
+    <mergeCell ref="H125:H127"/>
+    <mergeCell ref="B128:B131"/>
+    <mergeCell ref="C128:C131"/>
+    <mergeCell ref="G128:G131"/>
+    <mergeCell ref="H128:H131"/>
+    <mergeCell ref="B133:B143"/>
+    <mergeCell ref="C133:C143"/>
+    <mergeCell ref="F133:F143"/>
+    <mergeCell ref="G133:G143"/>
+    <mergeCell ref="B114:B117"/>
+    <mergeCell ref="F146:F149"/>
+    <mergeCell ref="G146:G149"/>
+    <mergeCell ref="B151:B152"/>
+    <mergeCell ref="C151:C152"/>
+    <mergeCell ref="D151:D152"/>
+    <mergeCell ref="F151:F152"/>
+    <mergeCell ref="G151:G152"/>
+    <mergeCell ref="G125:G127"/>
+    <mergeCell ref="B144:B145"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="C146:C149"/>
+    <mergeCell ref="E146:E149"/>
+    <mergeCell ref="H78:H79"/>
+    <mergeCell ref="B80:B87"/>
+    <mergeCell ref="B88:H88"/>
+    <mergeCell ref="B89:H89"/>
+    <mergeCell ref="B90:H90"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="H91:H94"/>
+    <mergeCell ref="B95:B105"/>
+    <mergeCell ref="E95:E105"/>
+    <mergeCell ref="C95:C105"/>
+    <mergeCell ref="F95:F105"/>
+    <mergeCell ref="G95:G105"/>
+    <mergeCell ref="B66:B70"/>
+    <mergeCell ref="F66:F70"/>
+    <mergeCell ref="G66:G70"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="F71:F74"/>
+    <mergeCell ref="G71:G74"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="B60:H60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="F61:F63"/>
+    <mergeCell ref="G61:G63"/>
+    <mergeCell ref="H61:H63"/>
+    <mergeCell ref="H52:H53"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="F54:F57"/>
+    <mergeCell ref="G54:G57"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="G44:G47"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="D32:D37"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="G18:G23"/>
+    <mergeCell ref="H18:H23"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
     <mergeCell ref="B160:B162"/>
     <mergeCell ref="C160:C162"/>
     <mergeCell ref="D160:D162"/>
@@ -35998,208 +36200,6 @@
     <mergeCell ref="C125:C127"/>
     <mergeCell ref="D125:D127"/>
     <mergeCell ref="B106:B113"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="F18:F23"/>
-    <mergeCell ref="G18:G23"/>
-    <mergeCell ref="H18:H23"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="D32:D37"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="G44:G47"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="H52:H53"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="E54:E57"/>
-    <mergeCell ref="F54:F57"/>
-    <mergeCell ref="G54:G57"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="B60:H60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="F61:F63"/>
-    <mergeCell ref="G61:G63"/>
-    <mergeCell ref="H61:H63"/>
-    <mergeCell ref="B66:B70"/>
-    <mergeCell ref="F66:F70"/>
-    <mergeCell ref="G66:G70"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="F71:F74"/>
-    <mergeCell ref="G71:G74"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="H78:H79"/>
-    <mergeCell ref="B80:B87"/>
-    <mergeCell ref="B88:H88"/>
-    <mergeCell ref="B89:H89"/>
-    <mergeCell ref="B90:H90"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="H91:H94"/>
-    <mergeCell ref="B95:B105"/>
-    <mergeCell ref="E95:E105"/>
-    <mergeCell ref="C95:C105"/>
-    <mergeCell ref="F95:F105"/>
-    <mergeCell ref="G95:G105"/>
-    <mergeCell ref="B114:B117"/>
-    <mergeCell ref="F146:F149"/>
-    <mergeCell ref="G146:G149"/>
-    <mergeCell ref="B151:B152"/>
-    <mergeCell ref="C151:C152"/>
-    <mergeCell ref="D151:D152"/>
-    <mergeCell ref="F151:F152"/>
-    <mergeCell ref="G151:G152"/>
-    <mergeCell ref="G125:G127"/>
-    <mergeCell ref="B144:B145"/>
-    <mergeCell ref="C144:C145"/>
-    <mergeCell ref="C146:C149"/>
-    <mergeCell ref="E146:E149"/>
-    <mergeCell ref="H125:H127"/>
-    <mergeCell ref="B128:B131"/>
-    <mergeCell ref="C128:C131"/>
-    <mergeCell ref="G128:G131"/>
-    <mergeCell ref="H128:H131"/>
-    <mergeCell ref="B133:B143"/>
-    <mergeCell ref="C133:C143"/>
-    <mergeCell ref="F133:F143"/>
-    <mergeCell ref="G133:G143"/>
-    <mergeCell ref="H151:H152"/>
-    <mergeCell ref="B153:H153"/>
-    <mergeCell ref="B154:H154"/>
-    <mergeCell ref="B155:H155"/>
-    <mergeCell ref="B156:B159"/>
-    <mergeCell ref="C156:C159"/>
-    <mergeCell ref="D156:D159"/>
-    <mergeCell ref="F156:F159"/>
-    <mergeCell ref="G156:G159"/>
-    <mergeCell ref="H156:H159"/>
-    <mergeCell ref="B168:H168"/>
-    <mergeCell ref="B169:B172"/>
-    <mergeCell ref="C169:C172"/>
-    <mergeCell ref="F169:F172"/>
-    <mergeCell ref="G169:G172"/>
-    <mergeCell ref="H169:H172"/>
-    <mergeCell ref="F164:F165"/>
-    <mergeCell ref="G164:G165"/>
-    <mergeCell ref="H164:H165"/>
-    <mergeCell ref="B166:H166"/>
-    <mergeCell ref="B167:H167"/>
-    <mergeCell ref="G174:G175"/>
-    <mergeCell ref="H174:H175"/>
-    <mergeCell ref="B176:B180"/>
-    <mergeCell ref="F176:F180"/>
-    <mergeCell ref="G176:G180"/>
-    <mergeCell ref="B174:B175"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="E174:E175"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="B187:H187"/>
-    <mergeCell ref="B188:H188"/>
-    <mergeCell ref="B189:B194"/>
-    <mergeCell ref="C189:C194"/>
-    <mergeCell ref="E189:E194"/>
-    <mergeCell ref="G189:G194"/>
-    <mergeCell ref="H189:H194"/>
-    <mergeCell ref="B181:B184"/>
-    <mergeCell ref="E181:E184"/>
-    <mergeCell ref="F181:F184"/>
-    <mergeCell ref="G181:G184"/>
-    <mergeCell ref="B186:H186"/>
-    <mergeCell ref="H196:H197"/>
-    <mergeCell ref="B198:H198"/>
-    <mergeCell ref="B199:H199"/>
-    <mergeCell ref="B200:H200"/>
-    <mergeCell ref="B201:B203"/>
-    <mergeCell ref="C201:C203"/>
-    <mergeCell ref="E201:E203"/>
-    <mergeCell ref="G201:G203"/>
-    <mergeCell ref="H201:H203"/>
-    <mergeCell ref="B196:B197"/>
-    <mergeCell ref="C196:C197"/>
-    <mergeCell ref="E196:E197"/>
-    <mergeCell ref="F196:F197"/>
-    <mergeCell ref="G196:G197"/>
-    <mergeCell ref="B204:H204"/>
-    <mergeCell ref="B205:H205"/>
-    <mergeCell ref="B206:H206"/>
-    <mergeCell ref="B208:B209"/>
-    <mergeCell ref="C208:C209"/>
-    <mergeCell ref="D208:D209"/>
-    <mergeCell ref="E208:E209"/>
-    <mergeCell ref="F208:F209"/>
-    <mergeCell ref="G208:G209"/>
-    <mergeCell ref="H208:H209"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" location="_ftn1" display="KOSOVO[1] DATA"/>
@@ -38534,7 +38534,7 @@
   <dimension ref="A1:S70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -39056,55 +39056,55 @@
       </c>
     </row>
     <row r="29" spans="2:17">
-      <c r="B29" s="167" t="s">
+      <c r="B29" s="121" t="s">
         <v>2460</v>
       </c>
-      <c r="E29" s="166">
+      <c r="E29" s="120">
         <f>E26/I35</f>
         <v>1.125</v>
       </c>
-      <c r="F29" s="166">
+      <c r="F29" s="120">
         <f t="shared" ref="F29:O29" si="1">F26/J35</f>
         <v>0.78145695364238421</v>
       </c>
-      <c r="G29" s="166">
+      <c r="G29" s="120">
         <f t="shared" si="1"/>
         <v>0.96610169491525422</v>
       </c>
-      <c r="H29" s="166">
+      <c r="H29" s="120">
         <f t="shared" si="1"/>
         <v>0.93958333333333333</v>
       </c>
-      <c r="I29" s="166">
+      <c r="I29" s="120">
         <f t="shared" si="1"/>
         <v>0.89916666666666656</v>
       </c>
-      <c r="J29" s="166">
+      <c r="J29" s="120">
         <f t="shared" si="1"/>
         <v>0.79279279279279291</v>
       </c>
-      <c r="K29" s="166">
+      <c r="K29" s="120">
         <f t="shared" si="1"/>
         <v>0.93814432989690721</v>
       </c>
-      <c r="L29" s="166">
+      <c r="L29" s="120">
         <f t="shared" si="1"/>
         <v>0.96969696969696961</v>
       </c>
-      <c r="M29" s="166">
+      <c r="M29" s="120">
         <f t="shared" si="1"/>
         <v>0.88749999999999984</v>
       </c>
-      <c r="N29" s="166">
+      <c r="N29" s="120">
         <f t="shared" si="1"/>
         <v>0.67938931297709926</v>
       </c>
-      <c r="O29" s="166">
+      <c r="O29" s="120">
         <f t="shared" si="1"/>
         <v>0.66754385964912277</v>
       </c>
-      <c r="P29" s="166"/>
-      <c r="Q29" s="166"/>
+      <c r="P29" s="120"/>
+      <c r="Q29" s="120"/>
     </row>
     <row r="31" spans="2:17" ht="20">
       <c r="B31" s="47" t="s">
@@ -39267,7 +39267,7 @@
       <c r="J36" s="70">
         <v>10.9</v>
       </c>
-      <c r="K36" s="169">
+      <c r="K36" s="123">
         <f>ROUND(K35*K40, 1)</f>
         <v>8.4</v>
       </c>
@@ -39283,18 +39283,18 @@
       <c r="O36" s="70">
         <v>7</v>
       </c>
-      <c r="P36" s="169">
+      <c r="P36" s="123">
         <f t="shared" ref="P36:Q36" si="2">ROUND(P35*P40, 1)</f>
         <v>7.6</v>
       </c>
-      <c r="Q36" s="169">
+      <c r="Q36" s="123">
         <f t="shared" si="2"/>
         <v>7.1</v>
       </c>
       <c r="R36" s="70">
         <v>11.1</v>
       </c>
-      <c r="S36" s="169">
+      <c r="S36" s="123">
         <f>ROUND(S35*S40, 1)</f>
         <v>9.6999999999999993</v>
       </c>
@@ -39468,7 +39468,7 @@
       </c>
     </row>
     <row r="40" spans="2:19">
-      <c r="B40" s="167" t="s">
+      <c r="B40" s="121" t="s">
         <v>2453</v>
       </c>
       <c r="C40" s="38"/>
@@ -39477,47 +39477,47 @@
       <c r="F40" s="38"/>
       <c r="G40" s="38"/>
       <c r="H40" s="38"/>
-      <c r="I40" s="166">
+      <c r="I40" s="120">
         <f>I36/I35</f>
         <v>0.7232142857142857</v>
       </c>
-      <c r="J40" s="166">
+      <c r="J40" s="120">
         <f>J36/J35</f>
         <v>0.72185430463576161</v>
       </c>
-      <c r="K40" s="168">
+      <c r="K40" s="122">
         <f>AVERAGE(J40,L40)</f>
         <v>0.71509381898454749</v>
       </c>
-      <c r="L40" s="166">
+      <c r="L40" s="120">
         <f>L36/L35</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="M40" s="166">
+      <c r="M40" s="120">
         <f>M36/M35</f>
         <v>0.73333333333333339</v>
       </c>
-      <c r="N40" s="166">
+      <c r="N40" s="120">
         <f>N36/N35</f>
         <v>0.83783783783783794</v>
       </c>
-      <c r="O40" s="166">
+      <c r="O40" s="120">
         <f>O36/O35</f>
         <v>0.72164948453608257</v>
       </c>
-      <c r="P40" s="168">
+      <c r="P40" s="122">
         <f>O40+((R40-O40)/3)</f>
         <v>0.76354240444899146</v>
       </c>
-      <c r="Q40" s="168">
+      <c r="Q40" s="122">
         <f>P40+((R40-O40)/3)</f>
         <v>0.80543532436190035</v>
       </c>
-      <c r="R40" s="166">
+      <c r="R40" s="120">
         <f>R36/R35</f>
         <v>0.84732824427480913</v>
       </c>
-      <c r="S40" s="168">
+      <c r="S40" s="122">
         <f>R40</f>
         <v>0.84732824427480913</v>
       </c>
@@ -39530,17 +39530,17 @@
       <c r="F41" s="38"/>
       <c r="G41" s="38"/>
       <c r="H41" s="38"/>
-      <c r="I41" s="166"/>
-      <c r="J41" s="166"/>
-      <c r="K41" s="166"/>
-      <c r="L41" s="166"/>
-      <c r="M41" s="166"/>
-      <c r="N41" s="166"/>
-      <c r="O41" s="166"/>
-      <c r="P41" s="166"/>
-      <c r="Q41" s="166"/>
-      <c r="R41" s="166"/>
-      <c r="S41" s="166"/>
+      <c r="I41" s="120"/>
+      <c r="J41" s="120"/>
+      <c r="K41" s="120"/>
+      <c r="L41" s="120"/>
+      <c r="M41" s="120"/>
+      <c r="N41" s="120"/>
+      <c r="O41" s="120"/>
+      <c r="P41" s="120"/>
+      <c r="Q41" s="120"/>
+      <c r="R41" s="120"/>
+      <c r="S41" s="120"/>
     </row>
     <row r="42" spans="2:19">
       <c r="D42" s="38"/>
@@ -40602,17 +40602,17 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="104" customHeight="1">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="169" t="s">
         <v>2212</v>
       </c>
-      <c r="C12" s="165"/>
-      <c r="D12" s="165"/>
-      <c r="E12" s="165"/>
-      <c r="F12" s="165"/>
-      <c r="G12" s="165"/>
-      <c r="H12" s="165"/>
-      <c r="I12" s="165"/>
-      <c r="J12" s="165"/>
+      <c r="C12" s="169"/>
+      <c r="D12" s="169"/>
+      <c r="E12" s="169"/>
+      <c r="F12" s="169"/>
+      <c r="G12" s="169"/>
+      <c r="H12" s="169"/>
+      <c r="I12" s="169"/>
+      <c r="J12" s="169"/>
     </row>
     <row r="13" spans="1:12">
       <c r="C13" s="49"/>

</xml_diff>